<commit_message>
PanelCentre by Perso + PanelInfoPoi
</commit_message>
<xml_diff>
--- a/LeTerrain-LeJeu/src/main/resources/fichiers/personnages.xlsx
+++ b/LeTerrain-LeJeu/src/main/resources/fichiers/personnages.xlsx
@@ -178,12 +178,6 @@
     <t>Darm, Tom, Darmch, Darmounich, De L'Armouni, De L'Harmonie</t>
   </si>
   <si>
-    <t>Pip, pipo, pips, pipas, pipouze, pieeeeerre, pierrot, pierrou, pierron, dj pierrot, les doigts de fer, la grosse bite</t>
-  </si>
-  <si>
-    <t>Nico, Nicou, Nicole, p'tit nain, Le p'tit pas beau, Le p'tit farfouilli au rapport, Le p'tit saoulant qui vient de fumer, Le p'tit grapineur</t>
-  </si>
-  <si>
     <t xml:space="preserve">Russ, Rush, Roych, Jo, Roychtipop, Roychtimole, </t>
   </si>
   <si>
@@ -583,6 +577,12 @@
   </si>
   <si>
     <t xml:space="preserve">est nerveux parce qu'il a un corps de lache et une narine qui part en couille, porte des lunettes de bigleux, fume comme un pd la main a plat, </t>
+  </si>
+  <si>
+    <t>Pip, pipo, pips, pipas, pipouze, pieeeeerre, pierrot, pierrou, pierron, pierre Bellemare, dj pierrot, les doigts de fer, la grosse bite</t>
+  </si>
+  <si>
+    <t>Nico, Nicou, Nipop, Nicole, p'tit nain, Le p'tit pas beau, Le p'tit farfouilli au rapport, Le p'tit saoulant qui vient de fumer, Le p'tit grapineur</t>
   </si>
 </sst>
 </file>
@@ -1242,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:K215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1293,7 +1293,7 @@
         <v>21</v>
       </c>
       <c r="K3" s="59" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="9" customFormat="1">
@@ -1361,22 +1361,22 @@
         <v>0</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>54</v>
+        <v>187</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>53</v>
+        <v>186</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>52</v>
@@ -1417,28 +1417,28 @@
         <v>1</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="F8" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="H8" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="16" t="s">
+      <c r="I8" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>63</v>
-      </c>
       <c r="J8" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K8" s="36"/>
     </row>
@@ -1447,28 +1447,28 @@
         <v>2</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G9" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>115</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>117</v>
       </c>
       <c r="K9" s="36"/>
     </row>
@@ -1477,28 +1477,28 @@
         <v>3</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I10" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="J10" s="18" t="s">
         <v>114</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>116</v>
       </c>
       <c r="K10" s="36"/>
     </row>
@@ -1507,28 +1507,28 @@
         <v>33</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D11" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>123</v>
-      </c>
       <c r="G11" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K11" s="36"/>
     </row>
@@ -1540,45 +1540,45 @@
       <c r="D12" s="12"/>
       <c r="E12" s="13"/>
       <c r="F12" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="16"/>
       <c r="I12" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K12" s="36"/>
     </row>
     <row r="13" spans="2:11" s="9" customFormat="1">
       <c r="B13" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="D13" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="G13" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>168</v>
-      </c>
       <c r="H13" s="16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K13" s="36"/>
     </row>
@@ -1587,19 +1587,19 @@
         <v>4</v>
       </c>
       <c r="C14" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="D14" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>172</v>
-      </c>
       <c r="G14" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H14" s="16" t="s">
         <v>43</v>
@@ -1608,7 +1608,7 @@
         <v>42</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K14" s="36"/>
     </row>
@@ -1629,10 +1629,10 @@
         <v>36</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="14" t="s">
@@ -1661,7 +1661,7 @@
       <c r="G17" s="15"/>
       <c r="H17" s="16"/>
       <c r="I17" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J17" s="18" t="s">
         <v>46</v>
@@ -1673,28 +1673,28 @@
         <v>38</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K18" s="36"/>
     </row>
@@ -1728,33 +1728,33 @@
       <c r="J20" s="18"/>
       <c r="K20" s="36"/>
     </row>
-    <row r="21" spans="2:11" s="9" customFormat="1" ht="75">
+    <row r="21" spans="2:11" s="9" customFormat="1" ht="60">
       <c r="B21" s="35" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F21" s="14" t="s">
         <v>50</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K21" s="36"/>
     </row>
@@ -1775,26 +1775,26 @@
         <v>35</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H23" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="J23" s="18" t="s">
         <v>134</v>
-      </c>
-      <c r="I23" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="J23" s="18" t="s">
-        <v>136</v>
       </c>
       <c r="K23" s="36"/>
     </row>
@@ -1812,39 +1812,39 @@
     </row>
     <row r="25" spans="2:11" s="9" customFormat="1" ht="30">
       <c r="B25" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D25" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="H25" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="F25" s="14" t="s">
+      <c r="I25" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="J25" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="G25" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="J25" s="18" t="s">
+      <c r="K25" s="36" t="s">
         <v>130</v>
-      </c>
-      <c r="K25" s="36" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="26" spans="2:11" s="9" customFormat="1">
       <c r="B26" s="35" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="19"/>
@@ -2136,7 +2136,7 @@
     </row>
     <row r="38" spans="2:11" s="9" customFormat="1">
       <c r="B38" s="35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="12"/>
@@ -2148,33 +2148,33 @@
       <c r="J38" s="18"/>
       <c r="K38" s="36"/>
     </row>
-    <row r="39" spans="2:11" s="9" customFormat="1" ht="30">
+    <row r="39" spans="2:11" s="9" customFormat="1">
       <c r="B39" s="37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C39" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H39" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="H39" s="16" t="s">
-        <v>79</v>
-      </c>
       <c r="I39" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K39" s="36"/>
     </row>
@@ -2192,29 +2192,29 @@
     </row>
     <row r="41" spans="2:11" s="9" customFormat="1">
       <c r="B41" s="35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="G41" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="H41" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="14" t="s">
+      <c r="I41" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="G41" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="H41" s="16" t="s">
+      <c r="J41" s="18" t="s">
         <v>85</v>
-      </c>
-      <c r="I41" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="J41" s="18" t="s">
-        <v>87</v>
       </c>
       <c r="K41" s="36"/>
     </row>
@@ -2232,31 +2232,31 @@
     </row>
     <row r="43" spans="2:11" s="9" customFormat="1" ht="45">
       <c r="B43" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="G43" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="I43" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="J43" s="18" t="s">
         <v>105</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="G43" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H43" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="I43" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="J43" s="18" t="s">
-        <v>107</v>
       </c>
       <c r="K43" s="36"/>
     </row>
@@ -2274,21 +2274,21 @@
     </row>
     <row r="45" spans="2:11" s="9" customFormat="1" ht="45">
       <c r="B45" s="35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E45" s="13"/>
       <c r="F45" s="14"/>
       <c r="G45" s="15"/>
       <c r="H45" s="16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I45" s="17"/>
       <c r="J45" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K45" s="36"/>
     </row>
@@ -2306,23 +2306,23 @@
     </row>
     <row r="47" spans="2:11" s="9" customFormat="1" ht="30">
       <c r="B47" s="35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C47" s="11"/>
       <c r="D47" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G47" s="15"/>
       <c r="H47" s="16"/>
       <c r="I47" s="17"/>
       <c r="J47" s="18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K47" s="36"/>
     </row>
@@ -2331,16 +2331,16 @@
       <c r="C48" s="11"/>
       <c r="D48" s="12"/>
       <c r="E48" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G48" s="15"/>
       <c r="H48" s="16"/>
       <c r="I48" s="17"/>
       <c r="J48" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K48" s="36"/>
     </row>
@@ -2349,16 +2349,16 @@
       <c r="C49" s="11"/>
       <c r="D49" s="12"/>
       <c r="E49" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G49" s="15"/>
       <c r="H49" s="16"/>
       <c r="I49" s="17"/>
       <c r="J49" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K49" s="36"/>
     </row>
@@ -2367,16 +2367,16 @@
       <c r="C50" s="11"/>
       <c r="D50" s="12"/>
       <c r="E50" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G50" s="15"/>
       <c r="H50" s="16"/>
       <c r="I50" s="17"/>
       <c r="J50" s="18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K50" s="36"/>
     </row>
@@ -2386,7 +2386,7 @@
       <c r="D51" s="12"/>
       <c r="E51" s="13"/>
       <c r="F51" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G51" s="15"/>
       <c r="H51" s="16"/>
@@ -2400,7 +2400,7 @@
       <c r="D52" s="12"/>
       <c r="E52" s="13"/>
       <c r="F52" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G52" s="15"/>
       <c r="H52" s="16"/>

</xml_diff>

<commit_message>
ActionCombat et missions pour Russ + Polices + Popos combat
</commit_message>
<xml_diff>
--- a/LeTerrain-LeJeu/src/main/resources/fichiers/personnages.xlsx
+++ b/LeTerrain-LeJeu/src/main/resources/fichiers/personnages.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19515" windowHeight="5220"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="18600" windowHeight="8595"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
   <oleSize ref="A1"/>
 </workbook>
 </file>
@@ -313,9 +313,6 @@
     <t>A vu la mere de Yo a poil</t>
   </si>
   <si>
-    <t>BoBSA66</t>
-  </si>
-  <si>
     <t>prise de l'etouffement jusqu'a mini-evanouite</t>
   </si>
   <si>
@@ -334,9 +331,6 @@
     <t>Un louveteau</t>
   </si>
   <si>
-    <t>Ne bois pas / Ne vomis plus depuis qu'il s'est rodé en Australie</t>
-  </si>
-  <si>
     <t>Ne vomis pas mais chie une fois tous les 5 jours</t>
   </si>
   <si>
@@ -365,9 +359,6 @@
   </si>
   <si>
     <t>starwars, nirvana, worms, crash lego,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le rhum de l'enculé de Pierre, le foot, jouer a croche mensonge, </t>
   </si>
   <si>
     <t>ingurgite, a des caillots dans la bite et des trous dans les cheveux, montre pas son cul mais sa bite, a eu un ongle de pied chocapic, ne finit pas un match de foot vivant</t>
@@ -380,9 +371,6 @@
     <t>foncde en soiree, connait Renaud, traine a la butte, se tape des moches/petites, a peur des serpents, ne crache pas dans les verres, mange des chocapic dans son slip</t>
   </si>
   <si>
-    <t xml:space="preserve">les voitures,  le sport, gueuler, mettre du minaves quand foncde, </t>
-  </si>
-  <si>
     <t>Lara Croft / Cyril Hanouna / Arthur</t>
   </si>
   <si>
@@ -583,6 +571,18 @@
   </si>
   <si>
     <t>aime se faire entourer de plastique fondu quand foncde, aime se faire fracasser le crane pour regarder le feu d'artifice par la fenetre, aime casser les radiateurs, aime sniffer du nez(j'ai gicle), aime se titiller la narine avec un cordon pour eternuer, aime le pain et le coca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le rhum de l'enculé de Pierre, le foot, world of warcraft, jouer a croche mensonge, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">les voitures,  le sport, gueuler, raler, rager, mettre du minaves quand foncde, </t>
+  </si>
+  <si>
+    <t>Ne bois pas, ne fume pas / Ne vomis plus depuis qu'il s'est rodé en Australie</t>
+  </si>
+  <si>
+    <t>808SA66</t>
   </si>
 </sst>
 </file>
@@ -1240,24 +1240,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:K215"/>
+  <dimension ref="B1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.375" customWidth="1"/>
-    <col min="3" max="3" width="24.375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="22.875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="22.875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="27.875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="23.375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.25" style="2" customWidth="1"/>
-    <col min="9" max="9" width="24.25" style="4" customWidth="1"/>
-    <col min="10" max="10" width="25.75" style="3" customWidth="1"/>
-    <col min="11" max="11" width="14.125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="61" customFormat="1">
@@ -1293,7 +1293,7 @@
         <v>21</v>
       </c>
       <c r="K3" s="59" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="9" customFormat="1">
@@ -1356,15 +1356,15 @@
       </c>
       <c r="K5" s="36"/>
     </row>
-    <row r="6" spans="2:11" s="9" customFormat="1" ht="75">
+    <row r="6" spans="2:11" s="9" customFormat="1" ht="105">
       <c r="B6" s="35" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>66</v>
@@ -1373,10 +1373,10 @@
         <v>53</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>52</v>
@@ -1442,97 +1442,97 @@
       </c>
       <c r="K8" s="36"/>
     </row>
-    <row r="9" spans="2:11" s="9" customFormat="1" ht="270">
+    <row r="9" spans="2:11" s="9" customFormat="1" ht="315">
       <c r="B9" s="35" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G9" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H9" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>114</v>
-      </c>
       <c r="K9" s="36"/>
     </row>
-    <row r="10" spans="2:11" s="9" customFormat="1" ht="105">
+    <row r="10" spans="2:11" s="9" customFormat="1" ht="120">
       <c r="B10" s="35" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I10" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="J10" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="J10" s="18" t="s">
-        <v>113</v>
-      </c>
       <c r="K10" s="36"/>
     </row>
-    <row r="11" spans="2:11" s="9" customFormat="1" ht="165">
+    <row r="11" spans="2:11" s="9" customFormat="1" ht="195">
       <c r="B11" s="35" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>116</v>
+        <v>184</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>120</v>
+        <v>185</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K11" s="36"/>
     </row>
-    <row r="12" spans="2:11" s="9" customFormat="1" ht="60">
+    <row r="12" spans="2:11" s="9" customFormat="1" ht="90">
       <c r="B12" s="35" t="s">
         <v>34</v>
       </c>
@@ -1540,66 +1540,66 @@
       <c r="D12" s="12"/>
       <c r="E12" s="13"/>
       <c r="F12" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="16"/>
       <c r="I12" s="17" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="K12" s="36"/>
     </row>
-    <row r="13" spans="2:11" s="9" customFormat="1">
+    <row r="13" spans="2:11" s="9" customFormat="1" ht="30">
       <c r="B13" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="G13" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>165</v>
-      </c>
       <c r="H13" s="16" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K13" s="36"/>
     </row>
-    <row r="14" spans="2:11" s="9" customFormat="1" ht="30">
+    <row r="14" spans="2:11" s="9" customFormat="1" ht="45">
       <c r="B14" s="35" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H14" s="16" t="s">
         <v>43</v>
@@ -1632,7 +1632,7 @@
         <v>86</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="14" t="s">
@@ -1661,14 +1661,14 @@
       <c r="G17" s="15"/>
       <c r="H17" s="16"/>
       <c r="I17" s="17" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J17" s="18" t="s">
         <v>46</v>
       </c>
       <c r="K17" s="36"/>
     </row>
-    <row r="18" spans="2:11" s="9" customFormat="1" ht="45">
+    <row r="18" spans="2:11" s="9" customFormat="1" ht="60">
       <c r="B18" s="35" t="s">
         <v>38</v>
       </c>
@@ -1676,25 +1676,25 @@
         <v>88</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="K18" s="36"/>
     </row>
@@ -1728,7 +1728,7 @@
       <c r="J20" s="18"/>
       <c r="K20" s="36"/>
     </row>
-    <row r="21" spans="2:11" s="9" customFormat="1" ht="60">
+    <row r="21" spans="2:11" s="9" customFormat="1" ht="75">
       <c r="B21" s="35" t="s">
         <v>41</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>64</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F21" s="14" t="s">
         <v>50</v>
@@ -1754,7 +1754,7 @@
         <v>63</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K21" s="36"/>
     </row>
@@ -1778,23 +1778,23 @@
         <v>87</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="14" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K23" s="36"/>
     </row>
@@ -1818,33 +1818,33 @@
         <v>88</v>
       </c>
       <c r="D25" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="I25" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="J25" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="K25" s="36" t="s">
         <v>125</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="J25" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="K25" s="36" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="26" spans="2:11" s="9" customFormat="1">
       <c r="B26" s="35" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="19"/>
@@ -1882,7 +1882,7 @@
       <c r="J28" s="18"/>
       <c r="K28" s="36"/>
     </row>
-    <row r="29" spans="2:11" s="9" customFormat="1">
+    <row r="29" spans="2:11" s="9" customFormat="1" ht="30">
       <c r="B29" s="35" t="s">
         <v>7</v>
       </c>
@@ -2002,7 +2002,7 @@
       </c>
       <c r="K32" s="36"/>
     </row>
-    <row r="33" spans="2:11" s="9" customFormat="1">
+    <row r="33" spans="2:11" s="9" customFormat="1" ht="30">
       <c r="B33" s="35" t="s">
         <v>12</v>
       </c>
@@ -2092,7 +2092,7 @@
       </c>
       <c r="K35" s="36"/>
     </row>
-    <row r="36" spans="2:11" s="9" customFormat="1">
+    <row r="36" spans="2:11" s="9" customFormat="1" ht="30">
       <c r="B36" s="35" t="s">
         <v>13</v>
       </c>
@@ -2148,7 +2148,7 @@
       <c r="J38" s="18"/>
       <c r="K38" s="36"/>
     </row>
-    <row r="39" spans="2:11" s="9" customFormat="1">
+    <row r="39" spans="2:11" s="9" customFormat="1" ht="30">
       <c r="B39" s="37" t="s">
         <v>68</v>
       </c>
@@ -2230,33 +2230,33 @@
       <c r="J42" s="63"/>
       <c r="K42" s="65"/>
     </row>
-    <row r="43" spans="2:11" s="9" customFormat="1" ht="45">
+    <row r="43" spans="2:11" s="9" customFormat="1" ht="60">
       <c r="B43" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D43" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C43" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D43" s="19" t="s">
+      <c r="E43" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="G43" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="I43" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="J43" s="18" t="s">
         <v>103</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="G43" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="H43" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="I43" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="J43" s="18" t="s">
-        <v>104</v>
       </c>
       <c r="K43" s="36"/>
     </row>
@@ -2284,11 +2284,11 @@
       <c r="F45" s="14"/>
       <c r="G45" s="15"/>
       <c r="H45" s="16" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I45" s="17"/>
       <c r="J45" s="18" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K45" s="36"/>
     </row>
@@ -2304,7 +2304,7 @@
       <c r="J46" s="63"/>
       <c r="K46" s="65"/>
     </row>
-    <row r="47" spans="2:11" s="9" customFormat="1" ht="30">
+    <row r="47" spans="2:11" s="9" customFormat="1" ht="45">
       <c r="B47" s="35" t="s">
         <v>89</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>96</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F47" s="14" t="s">
         <v>92</v>
@@ -2331,7 +2331,7 @@
       <c r="C48" s="11"/>
       <c r="D48" s="12"/>
       <c r="E48" s="13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F48" s="14" t="s">
         <v>93</v>
@@ -2340,7 +2340,7 @@
       <c r="H48" s="16"/>
       <c r="I48" s="17"/>
       <c r="J48" s="18" t="s">
-        <v>98</v>
+        <v>187</v>
       </c>
       <c r="K48" s="36"/>
     </row>
@@ -2349,7 +2349,7 @@
       <c r="C49" s="11"/>
       <c r="D49" s="12"/>
       <c r="E49" s="13" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F49" s="14" t="s">
         <v>90</v>
@@ -2358,16 +2358,16 @@
       <c r="H49" s="16"/>
       <c r="I49" s="17"/>
       <c r="J49" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K49" s="36"/>
     </row>
-    <row r="50" spans="2:11" s="9" customFormat="1" ht="75">
+    <row r="50" spans="2:11" s="9" customFormat="1" ht="90">
       <c r="B50" s="35"/>
       <c r="C50" s="11"/>
       <c r="D50" s="12"/>
       <c r="E50" s="13" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F50" s="14" t="s">
         <v>91</v>
@@ -2376,7 +2376,7 @@
       <c r="H50" s="16"/>
       <c r="I50" s="17"/>
       <c r="J50" s="18" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="K50" s="36"/>
     </row>
@@ -2386,7 +2386,7 @@
       <c r="D51" s="12"/>
       <c r="E51" s="13"/>
       <c r="F51" s="14" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G51" s="15"/>
       <c r="H51" s="16"/>
@@ -2400,7 +2400,7 @@
       <c r="D52" s="12"/>
       <c r="E52" s="13"/>
       <c r="F52" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G52" s="15"/>
       <c r="H52" s="16"/>
@@ -2504,7 +2504,7 @@
       <c r="J60" s="18"/>
       <c r="K60" s="36"/>
     </row>
-    <row r="61" spans="2:11" customFormat="1">
+    <row r="61" spans="2:11">
       <c r="B61" s="38"/>
       <c r="C61" s="27"/>
       <c r="D61" s="28"/>
@@ -2516,7 +2516,7 @@
       <c r="J61" s="34"/>
       <c r="K61" s="39"/>
     </row>
-    <row r="62" spans="2:11" customFormat="1">
+    <row r="62" spans="2:11">
       <c r="B62" s="38"/>
       <c r="C62" s="27"/>
       <c r="D62" s="28"/>
@@ -2528,7 +2528,7 @@
       <c r="J62" s="34"/>
       <c r="K62" s="39"/>
     </row>
-    <row r="63" spans="2:11" customFormat="1">
+    <row r="63" spans="2:11">
       <c r="B63" s="38"/>
       <c r="C63" s="27"/>
       <c r="D63" s="28"/>
@@ -2540,7 +2540,7 @@
       <c r="J63" s="34"/>
       <c r="K63" s="39"/>
     </row>
-    <row r="64" spans="2:11" customFormat="1">
+    <row r="64" spans="2:11">
       <c r="B64" s="38"/>
       <c r="C64" s="27"/>
       <c r="D64" s="28"/>
@@ -2552,7 +2552,7 @@
       <c r="J64" s="34"/>
       <c r="K64" s="39"/>
     </row>
-    <row r="65" spans="2:11" customFormat="1">
+    <row r="65" spans="2:11">
       <c r="B65" s="38"/>
       <c r="C65" s="27"/>
       <c r="D65" s="28"/>
@@ -2564,7 +2564,7 @@
       <c r="J65" s="34"/>
       <c r="K65" s="39"/>
     </row>
-    <row r="66" spans="2:11" customFormat="1">
+    <row r="66" spans="2:11">
       <c r="B66" s="38"/>
       <c r="C66" s="27"/>
       <c r="D66" s="28"/>
@@ -2576,7 +2576,7 @@
       <c r="J66" s="34"/>
       <c r="K66" s="39"/>
     </row>
-    <row r="67" spans="2:11" customFormat="1">
+    <row r="67" spans="2:11">
       <c r="B67" s="38"/>
       <c r="C67" s="27"/>
       <c r="D67" s="28"/>
@@ -2588,7 +2588,7 @@
       <c r="J67" s="34"/>
       <c r="K67" s="39"/>
     </row>
-    <row r="68" spans="2:11" customFormat="1">
+    <row r="68" spans="2:11">
       <c r="B68" s="38"/>
       <c r="C68" s="27"/>
       <c r="D68" s="28"/>
@@ -2600,7 +2600,7 @@
       <c r="J68" s="34"/>
       <c r="K68" s="39"/>
     </row>
-    <row r="69" spans="2:11" customFormat="1">
+    <row r="69" spans="2:11">
       <c r="B69" s="38"/>
       <c r="C69" s="27"/>
       <c r="D69" s="28"/>
@@ -2612,7 +2612,7 @@
       <c r="J69" s="34"/>
       <c r="K69" s="39"/>
     </row>
-    <row r="70" spans="2:11" customFormat="1" ht="15.75" thickBot="1">
+    <row r="70" spans="2:11" ht="15.75" thickBot="1">
       <c r="B70" s="40"/>
       <c r="C70" s="41"/>
       <c r="D70" s="42"/>
@@ -2623,1425 +2623,6 @@
       <c r="I70" s="47"/>
       <c r="J70" s="48"/>
       <c r="K70" s="49"/>
-    </row>
-    <row r="71" spans="2:11" customFormat="1">
-      <c r="C71" s="7"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="8"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="3"/>
-      <c r="K71" s="10"/>
-    </row>
-    <row r="72" spans="2:11" customFormat="1">
-      <c r="C72" s="7"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="8"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="4"/>
-      <c r="J72" s="3"/>
-      <c r="K72" s="10"/>
-    </row>
-    <row r="73" spans="2:11" customFormat="1">
-      <c r="C73" s="7"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="8"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="3"/>
-      <c r="K73" s="10"/>
-    </row>
-    <row r="74" spans="2:11" customFormat="1">
-      <c r="C74" s="7"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="8"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="4"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="10"/>
-    </row>
-    <row r="78" spans="2:11" customFormat="1">
-      <c r="C78" s="7"/>
-      <c r="D78" s="6"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="8"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="3"/>
-      <c r="K78" s="10"/>
-    </row>
-    <row r="79" spans="2:11" customFormat="1">
-      <c r="C79" s="7"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="5"/>
-      <c r="F79" s="8"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="4"/>
-      <c r="J79" s="3"/>
-      <c r="K79" s="10"/>
-    </row>
-    <row r="80" spans="2:11" customFormat="1">
-      <c r="C80" s="7"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="8"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="4"/>
-      <c r="J80" s="3"/>
-      <c r="K80" s="10"/>
-    </row>
-    <row r="81" spans="2:11" customFormat="1">
-      <c r="C81" s="7"/>
-      <c r="D81" s="6"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="8"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="2"/>
-      <c r="I81" s="4"/>
-      <c r="J81" s="3"/>
-      <c r="K81" s="10"/>
-    </row>
-    <row r="82" spans="2:11" customFormat="1">
-      <c r="C82" s="7"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="8"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="4"/>
-      <c r="J82" s="3"/>
-      <c r="K82" s="10"/>
-    </row>
-    <row r="83" spans="2:11" customFormat="1">
-      <c r="C83" s="7"/>
-      <c r="D83" s="6"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="8"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="2"/>
-      <c r="I83" s="4"/>
-      <c r="J83" s="3"/>
-      <c r="K83" s="10"/>
-    </row>
-    <row r="84" spans="2:11" customFormat="1">
-      <c r="C84" s="7"/>
-      <c r="D84" s="6"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="8"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="4"/>
-      <c r="J84" s="3"/>
-      <c r="K84" s="10"/>
-    </row>
-    <row r="85" spans="2:11" customFormat="1">
-      <c r="C85" s="7"/>
-      <c r="D85" s="6"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="8"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="4"/>
-      <c r="J85" s="3"/>
-      <c r="K85" s="10"/>
-    </row>
-    <row r="86" spans="2:11" customFormat="1">
-      <c r="C86" s="7"/>
-      <c r="D86" s="6"/>
-      <c r="E86" s="5"/>
-      <c r="F86" s="8"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="4"/>
-      <c r="J86" s="3"/>
-      <c r="K86" s="10"/>
-    </row>
-    <row r="87" spans="2:11" customFormat="1">
-      <c r="C87" s="7"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="5"/>
-      <c r="F87" s="8"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="2"/>
-      <c r="I87" s="4"/>
-      <c r="J87" s="3"/>
-      <c r="K87" s="10"/>
-    </row>
-    <row r="88" spans="2:11" customFormat="1">
-      <c r="C88" s="7"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="8"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="4"/>
-      <c r="J88" s="3"/>
-      <c r="K88" s="10"/>
-    </row>
-    <row r="89" spans="2:11" customFormat="1">
-      <c r="C89" s="7"/>
-      <c r="D89" s="6"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="8"/>
-      <c r="G89" s="1"/>
-      <c r="H89" s="2"/>
-      <c r="I89" s="4"/>
-      <c r="J89" s="3"/>
-      <c r="K89" s="10"/>
-    </row>
-    <row r="90" spans="2:11" customFormat="1">
-      <c r="C90" s="7"/>
-      <c r="D90" s="6"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="8"/>
-      <c r="G90" s="1"/>
-      <c r="H90" s="2"/>
-      <c r="I90" s="4"/>
-      <c r="J90" s="3"/>
-      <c r="K90" s="10"/>
-    </row>
-    <row r="91" spans="2:11" customFormat="1">
-      <c r="C91" s="7"/>
-      <c r="D91" s="6"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="8"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="2"/>
-      <c r="I91" s="4"/>
-      <c r="J91" s="3"/>
-      <c r="K91" s="10"/>
-    </row>
-    <row r="92" spans="2:11" customFormat="1">
-      <c r="C92" s="7"/>
-      <c r="D92" s="6"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="8"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="2"/>
-      <c r="I92" s="4"/>
-      <c r="J92" s="3"/>
-      <c r="K92" s="10"/>
-    </row>
-    <row r="93" spans="2:11" customFormat="1">
-      <c r="C93" s="7"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="5"/>
-      <c r="F93" s="8"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="2"/>
-      <c r="I93" s="4"/>
-      <c r="J93" s="3"/>
-      <c r="K93" s="10"/>
-    </row>
-    <row r="94" spans="2:11" customFormat="1">
-      <c r="C94" s="7"/>
-      <c r="D94" s="6"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="8"/>
-      <c r="G94" s="1"/>
-      <c r="H94" s="2"/>
-      <c r="I94" s="4"/>
-      <c r="J94" s="3"/>
-      <c r="K94" s="10"/>
-    </row>
-    <row r="95" spans="2:11" customFormat="1">
-      <c r="C95" s="7"/>
-      <c r="D95" s="6"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="8"/>
-      <c r="G95" s="1"/>
-      <c r="H95" s="2"/>
-      <c r="I95" s="4"/>
-      <c r="J95" s="3"/>
-      <c r="K95" s="10"/>
-    </row>
-    <row r="96" spans="2:11" customFormat="1">
-      <c r="C96" s="7"/>
-      <c r="D96" s="6"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="8"/>
-      <c r="G96" s="1"/>
-      <c r="H96" s="2"/>
-      <c r="I96" s="4"/>
-      <c r="J96" s="3"/>
-      <c r="K96" s="10"/>
-    </row>
-    <row r="97" spans="2:11" customFormat="1">
-      <c r="C97" s="7"/>
-      <c r="D97" s="6"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="8"/>
-      <c r="G97" s="1"/>
-      <c r="H97" s="2"/>
-      <c r="I97" s="4"/>
-      <c r="J97" s="3"/>
-      <c r="K97" s="10"/>
-    </row>
-    <row r="98" spans="2:11" customFormat="1">
-      <c r="C98" s="7"/>
-      <c r="D98" s="6"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="8"/>
-      <c r="G98" s="1"/>
-      <c r="H98" s="2"/>
-      <c r="I98" s="4"/>
-      <c r="J98" s="3"/>
-      <c r="K98" s="10"/>
-    </row>
-    <row r="99" spans="2:11" customFormat="1">
-      <c r="C99" s="7"/>
-      <c r="D99" s="6"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="8"/>
-      <c r="G99" s="1"/>
-      <c r="H99" s="2"/>
-      <c r="I99" s="4"/>
-      <c r="J99" s="3"/>
-      <c r="K99" s="10"/>
-    </row>
-    <row r="100" spans="2:11" customFormat="1">
-      <c r="C100" s="7"/>
-      <c r="D100" s="6"/>
-      <c r="E100" s="5"/>
-      <c r="F100" s="8"/>
-      <c r="G100" s="1"/>
-      <c r="H100" s="2"/>
-      <c r="I100" s="4"/>
-      <c r="J100" s="3"/>
-      <c r="K100" s="10"/>
-    </row>
-    <row r="101" spans="2:11" customFormat="1">
-      <c r="C101" s="7"/>
-      <c r="D101" s="6"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="8"/>
-      <c r="G101" s="1"/>
-      <c r="H101" s="2"/>
-      <c r="I101" s="4"/>
-      <c r="J101" s="3"/>
-      <c r="K101" s="10"/>
-    </row>
-    <row r="102" spans="2:11" customFormat="1">
-      <c r="C102" s="7"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="8"/>
-      <c r="G102" s="1"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="4"/>
-      <c r="J102" s="3"/>
-      <c r="K102" s="10"/>
-    </row>
-    <row r="103" spans="2:11" customFormat="1">
-      <c r="C103" s="7"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="8"/>
-      <c r="G103" s="1"/>
-      <c r="H103" s="2"/>
-      <c r="I103" s="4"/>
-      <c r="J103" s="3"/>
-      <c r="K103" s="10"/>
-    </row>
-    <row r="104" spans="2:11" customFormat="1">
-      <c r="C104" s="7"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="8"/>
-      <c r="G104" s="1"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="4"/>
-      <c r="J104" s="3"/>
-      <c r="K104" s="10"/>
-    </row>
-    <row r="105" spans="2:11" customFormat="1">
-      <c r="C105" s="7"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="5"/>
-      <c r="F105" s="8"/>
-      <c r="G105" s="1"/>
-      <c r="H105" s="2"/>
-      <c r="I105" s="4"/>
-      <c r="J105" s="3"/>
-      <c r="K105" s="10"/>
-    </row>
-    <row r="106" spans="2:11" customFormat="1">
-      <c r="C106" s="7"/>
-      <c r="D106" s="6"/>
-      <c r="E106" s="5"/>
-      <c r="F106" s="8"/>
-      <c r="G106" s="1"/>
-      <c r="H106" s="2"/>
-      <c r="I106" s="4"/>
-      <c r="J106" s="3"/>
-      <c r="K106" s="10"/>
-    </row>
-    <row r="107" spans="2:11" customFormat="1">
-      <c r="C107" s="7"/>
-      <c r="D107" s="6"/>
-      <c r="E107" s="5"/>
-      <c r="F107" s="8"/>
-      <c r="G107" s="1"/>
-      <c r="H107" s="2"/>
-      <c r="I107" s="4"/>
-      <c r="J107" s="3"/>
-      <c r="K107" s="10"/>
-    </row>
-    <row r="108" spans="2:11" customFormat="1">
-      <c r="C108" s="7"/>
-      <c r="D108" s="6"/>
-      <c r="E108" s="5"/>
-      <c r="F108" s="8"/>
-      <c r="G108" s="1"/>
-      <c r="H108" s="2"/>
-      <c r="I108" s="4"/>
-      <c r="J108" s="3"/>
-      <c r="K108" s="10"/>
-    </row>
-    <row r="109" spans="2:11" customFormat="1">
-      <c r="C109" s="7"/>
-      <c r="D109" s="6"/>
-      <c r="E109" s="5"/>
-      <c r="F109" s="8"/>
-      <c r="G109" s="1"/>
-      <c r="H109" s="2"/>
-      <c r="I109" s="4"/>
-      <c r="J109" s="3"/>
-      <c r="K109" s="10"/>
-    </row>
-    <row r="110" spans="2:11" customFormat="1">
-      <c r="C110" s="7"/>
-      <c r="D110" s="6"/>
-      <c r="E110" s="5"/>
-      <c r="F110" s="8"/>
-      <c r="G110" s="1"/>
-      <c r="H110" s="2"/>
-      <c r="I110" s="4"/>
-      <c r="J110" s="3"/>
-      <c r="K110" s="10"/>
-    </row>
-    <row r="111" spans="2:11" customFormat="1">
-      <c r="C111" s="7"/>
-      <c r="D111" s="6"/>
-      <c r="E111" s="5"/>
-      <c r="F111" s="8"/>
-      <c r="G111" s="1"/>
-      <c r="H111" s="2"/>
-      <c r="I111" s="4"/>
-      <c r="J111" s="3"/>
-      <c r="K111" s="10"/>
-    </row>
-    <row r="112" spans="2:11" customFormat="1">
-      <c r="C112" s="7"/>
-      <c r="D112" s="6"/>
-      <c r="E112" s="5"/>
-      <c r="F112" s="8"/>
-      <c r="G112" s="1"/>
-      <c r="H112" s="2"/>
-      <c r="I112" s="4"/>
-      <c r="J112" s="3"/>
-      <c r="K112" s="10"/>
-    </row>
-    <row r="113" spans="2:11" customFormat="1">
-      <c r="C113" s="7"/>
-      <c r="D113" s="6"/>
-      <c r="E113" s="5"/>
-      <c r="F113" s="8"/>
-      <c r="G113" s="1"/>
-      <c r="H113" s="2"/>
-      <c r="I113" s="4"/>
-      <c r="J113" s="3"/>
-      <c r="K113" s="10"/>
-    </row>
-    <row r="114" spans="2:11" customFormat="1">
-      <c r="C114" s="7"/>
-      <c r="D114" s="6"/>
-      <c r="E114" s="5"/>
-      <c r="F114" s="8"/>
-      <c r="G114" s="1"/>
-      <c r="H114" s="2"/>
-      <c r="I114" s="4"/>
-      <c r="J114" s="3"/>
-      <c r="K114" s="10"/>
-    </row>
-    <row r="115" spans="2:11" customFormat="1">
-      <c r="C115" s="7"/>
-      <c r="D115" s="6"/>
-      <c r="E115" s="5"/>
-      <c r="F115" s="8"/>
-      <c r="G115" s="1"/>
-      <c r="H115" s="2"/>
-      <c r="I115" s="4"/>
-      <c r="J115" s="3"/>
-      <c r="K115" s="10"/>
-    </row>
-    <row r="116" spans="2:11" customFormat="1">
-      <c r="C116" s="7"/>
-      <c r="D116" s="6"/>
-      <c r="E116" s="5"/>
-      <c r="F116" s="8"/>
-      <c r="G116" s="1"/>
-      <c r="H116" s="2"/>
-      <c r="I116" s="4"/>
-      <c r="J116" s="3"/>
-      <c r="K116" s="10"/>
-    </row>
-    <row r="117" spans="2:11" customFormat="1">
-      <c r="C117" s="7"/>
-      <c r="D117" s="6"/>
-      <c r="E117" s="5"/>
-      <c r="F117" s="8"/>
-      <c r="G117" s="1"/>
-      <c r="H117" s="2"/>
-      <c r="I117" s="4"/>
-      <c r="J117" s="3"/>
-      <c r="K117" s="10"/>
-    </row>
-    <row r="118" spans="2:11" customFormat="1">
-      <c r="C118" s="7"/>
-      <c r="D118" s="6"/>
-      <c r="E118" s="5"/>
-      <c r="F118" s="8"/>
-      <c r="G118" s="1"/>
-      <c r="H118" s="2"/>
-      <c r="I118" s="4"/>
-      <c r="J118" s="3"/>
-      <c r="K118" s="10"/>
-    </row>
-    <row r="119" spans="2:11" customFormat="1">
-      <c r="C119" s="7"/>
-      <c r="D119" s="6"/>
-      <c r="E119" s="5"/>
-      <c r="F119" s="8"/>
-      <c r="G119" s="1"/>
-      <c r="H119" s="2"/>
-      <c r="I119" s="4"/>
-      <c r="J119" s="3"/>
-      <c r="K119" s="10"/>
-    </row>
-    <row r="120" spans="2:11" customFormat="1">
-      <c r="C120" s="7"/>
-      <c r="D120" s="6"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="8"/>
-      <c r="G120" s="1"/>
-      <c r="H120" s="2"/>
-      <c r="I120" s="4"/>
-      <c r="J120" s="3"/>
-      <c r="K120" s="10"/>
-    </row>
-    <row r="121" spans="2:11" customFormat="1">
-      <c r="C121" s="7"/>
-      <c r="D121" s="6"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="8"/>
-      <c r="G121" s="1"/>
-      <c r="H121" s="2"/>
-      <c r="I121" s="4"/>
-      <c r="J121" s="3"/>
-      <c r="K121" s="10"/>
-    </row>
-    <row r="122" spans="2:11" customFormat="1">
-      <c r="C122" s="7"/>
-      <c r="D122" s="6"/>
-      <c r="E122" s="5"/>
-      <c r="F122" s="8"/>
-      <c r="G122" s="1"/>
-      <c r="H122" s="2"/>
-      <c r="I122" s="4"/>
-      <c r="J122" s="3"/>
-      <c r="K122" s="10"/>
-    </row>
-    <row r="123" spans="2:11" customFormat="1">
-      <c r="C123" s="7"/>
-      <c r="D123" s="6"/>
-      <c r="E123" s="5"/>
-      <c r="F123" s="8"/>
-      <c r="G123" s="1"/>
-      <c r="H123" s="2"/>
-      <c r="I123" s="4"/>
-      <c r="J123" s="3"/>
-      <c r="K123" s="10"/>
-    </row>
-    <row r="124" spans="2:11" customFormat="1">
-      <c r="C124" s="7"/>
-      <c r="D124" s="6"/>
-      <c r="E124" s="5"/>
-      <c r="F124" s="8"/>
-      <c r="G124" s="1"/>
-      <c r="H124" s="2"/>
-      <c r="I124" s="4"/>
-      <c r="J124" s="3"/>
-      <c r="K124" s="10"/>
-    </row>
-    <row r="125" spans="2:11" customFormat="1">
-      <c r="C125" s="7"/>
-      <c r="D125" s="6"/>
-      <c r="E125" s="5"/>
-      <c r="F125" s="8"/>
-      <c r="G125" s="1"/>
-      <c r="H125" s="2"/>
-      <c r="I125" s="4"/>
-      <c r="J125" s="3"/>
-      <c r="K125" s="10"/>
-    </row>
-    <row r="126" spans="2:11" customFormat="1">
-      <c r="C126" s="7"/>
-      <c r="D126" s="6"/>
-      <c r="E126" s="5"/>
-      <c r="F126" s="8"/>
-      <c r="G126" s="1"/>
-      <c r="H126" s="2"/>
-      <c r="I126" s="4"/>
-      <c r="J126" s="3"/>
-      <c r="K126" s="10"/>
-    </row>
-    <row r="127" spans="2:11" customFormat="1">
-      <c r="C127" s="7"/>
-      <c r="D127" s="6"/>
-      <c r="E127" s="5"/>
-      <c r="F127" s="8"/>
-      <c r="G127" s="1"/>
-      <c r="H127" s="2"/>
-      <c r="I127" s="4"/>
-      <c r="J127" s="3"/>
-      <c r="K127" s="10"/>
-    </row>
-    <row r="128" spans="2:11" customFormat="1">
-      <c r="C128" s="7"/>
-      <c r="D128" s="6"/>
-      <c r="E128" s="5"/>
-      <c r="F128" s="8"/>
-      <c r="G128" s="1"/>
-      <c r="H128" s="2"/>
-      <c r="I128" s="4"/>
-      <c r="J128" s="3"/>
-      <c r="K128" s="10"/>
-    </row>
-    <row r="129" spans="2:11" customFormat="1">
-      <c r="C129" s="7"/>
-      <c r="D129" s="6"/>
-      <c r="E129" s="5"/>
-      <c r="F129" s="8"/>
-      <c r="G129" s="1"/>
-      <c r="H129" s="2"/>
-      <c r="I129" s="4"/>
-      <c r="J129" s="3"/>
-      <c r="K129" s="10"/>
-    </row>
-    <row r="130" spans="2:11" customFormat="1">
-      <c r="C130" s="7"/>
-      <c r="D130" s="6"/>
-      <c r="E130" s="5"/>
-      <c r="F130" s="8"/>
-      <c r="G130" s="1"/>
-      <c r="H130" s="2"/>
-      <c r="I130" s="4"/>
-      <c r="J130" s="3"/>
-      <c r="K130" s="10"/>
-    </row>
-    <row r="131" spans="2:11" customFormat="1">
-      <c r="C131" s="7"/>
-      <c r="D131" s="6"/>
-      <c r="E131" s="5"/>
-      <c r="F131" s="8"/>
-      <c r="G131" s="1"/>
-      <c r="H131" s="2"/>
-      <c r="I131" s="4"/>
-      <c r="J131" s="3"/>
-      <c r="K131" s="10"/>
-    </row>
-    <row r="132" spans="2:11" customFormat="1">
-      <c r="C132" s="7"/>
-      <c r="D132" s="6"/>
-      <c r="E132" s="5"/>
-      <c r="F132" s="8"/>
-      <c r="G132" s="1"/>
-      <c r="H132" s="2"/>
-      <c r="I132" s="4"/>
-      <c r="J132" s="3"/>
-      <c r="K132" s="10"/>
-    </row>
-    <row r="133" spans="2:11" customFormat="1">
-      <c r="C133" s="7"/>
-      <c r="D133" s="6"/>
-      <c r="E133" s="5"/>
-      <c r="F133" s="8"/>
-      <c r="G133" s="1"/>
-      <c r="H133" s="2"/>
-      <c r="I133" s="4"/>
-      <c r="J133" s="3"/>
-      <c r="K133" s="10"/>
-    </row>
-    <row r="134" spans="2:11" customFormat="1">
-      <c r="C134" s="7"/>
-      <c r="D134" s="6"/>
-      <c r="E134" s="5"/>
-      <c r="F134" s="8"/>
-      <c r="G134" s="1"/>
-      <c r="H134" s="2"/>
-      <c r="I134" s="4"/>
-      <c r="J134" s="3"/>
-      <c r="K134" s="10"/>
-    </row>
-    <row r="135" spans="2:11" customFormat="1">
-      <c r="C135" s="7"/>
-      <c r="D135" s="6"/>
-      <c r="E135" s="5"/>
-      <c r="F135" s="8"/>
-      <c r="G135" s="1"/>
-      <c r="H135" s="2"/>
-      <c r="I135" s="4"/>
-      <c r="J135" s="3"/>
-      <c r="K135" s="10"/>
-    </row>
-    <row r="137" spans="2:11" customFormat="1">
-      <c r="C137" s="7"/>
-      <c r="D137" s="6"/>
-      <c r="E137" s="5"/>
-      <c r="F137" s="8"/>
-      <c r="G137" s="1"/>
-      <c r="H137" s="2"/>
-      <c r="I137" s="4"/>
-      <c r="J137" s="3"/>
-      <c r="K137" s="10"/>
-    </row>
-    <row r="138" spans="2:11" customFormat="1">
-      <c r="C138" s="7"/>
-      <c r="D138" s="6"/>
-      <c r="E138" s="5"/>
-      <c r="F138" s="8"/>
-      <c r="G138" s="1"/>
-      <c r="H138" s="2"/>
-      <c r="I138" s="4"/>
-      <c r="J138" s="3"/>
-      <c r="K138" s="10"/>
-    </row>
-    <row r="139" spans="2:11" customFormat="1">
-      <c r="C139" s="7"/>
-      <c r="D139" s="6"/>
-      <c r="E139" s="5"/>
-      <c r="F139" s="8"/>
-      <c r="G139" s="1"/>
-      <c r="H139" s="2"/>
-      <c r="I139" s="4"/>
-      <c r="J139" s="3"/>
-      <c r="K139" s="10"/>
-    </row>
-    <row r="140" spans="2:11" customFormat="1">
-      <c r="C140" s="7"/>
-      <c r="D140" s="6"/>
-      <c r="E140" s="5"/>
-      <c r="F140" s="8"/>
-      <c r="G140" s="1"/>
-      <c r="H140" s="2"/>
-      <c r="I140" s="4"/>
-      <c r="J140" s="3"/>
-      <c r="K140" s="10"/>
-    </row>
-    <row r="141" spans="2:11" customFormat="1">
-      <c r="C141" s="7"/>
-      <c r="D141" s="6"/>
-      <c r="E141" s="5"/>
-      <c r="F141" s="8"/>
-      <c r="G141" s="1"/>
-      <c r="H141" s="2"/>
-      <c r="I141" s="4"/>
-      <c r="J141" s="3"/>
-      <c r="K141" s="10"/>
-    </row>
-    <row r="142" spans="2:11" customFormat="1">
-      <c r="C142" s="7"/>
-      <c r="D142" s="6"/>
-      <c r="E142" s="5"/>
-      <c r="F142" s="8"/>
-      <c r="G142" s="1"/>
-      <c r="H142" s="2"/>
-      <c r="I142" s="4"/>
-      <c r="J142" s="3"/>
-      <c r="K142" s="10"/>
-    </row>
-    <row r="143" spans="2:11" customFormat="1">
-      <c r="C143" s="7"/>
-      <c r="D143" s="6"/>
-      <c r="E143" s="5"/>
-      <c r="F143" s="8"/>
-      <c r="G143" s="1"/>
-      <c r="H143" s="2"/>
-      <c r="I143" s="4"/>
-      <c r="J143" s="3"/>
-      <c r="K143" s="10"/>
-    </row>
-    <row r="144" spans="2:11" customFormat="1">
-      <c r="C144" s="7"/>
-      <c r="D144" s="6"/>
-      <c r="E144" s="5"/>
-      <c r="F144" s="8"/>
-      <c r="G144" s="1"/>
-      <c r="H144" s="2"/>
-      <c r="I144" s="4"/>
-      <c r="J144" s="3"/>
-      <c r="K144" s="10"/>
-    </row>
-    <row r="145" spans="2:11" customFormat="1">
-      <c r="C145" s="7"/>
-      <c r="D145" s="6"/>
-      <c r="E145" s="5"/>
-      <c r="F145" s="8"/>
-      <c r="G145" s="1"/>
-      <c r="H145" s="2"/>
-      <c r="I145" s="4"/>
-      <c r="J145" s="3"/>
-      <c r="K145" s="10"/>
-    </row>
-    <row r="146" spans="2:11" customFormat="1">
-      <c r="C146" s="7"/>
-      <c r="D146" s="6"/>
-      <c r="E146" s="5"/>
-      <c r="F146" s="8"/>
-      <c r="G146" s="1"/>
-      <c r="H146" s="2"/>
-      <c r="I146" s="4"/>
-      <c r="J146" s="3"/>
-      <c r="K146" s="10"/>
-    </row>
-    <row r="147" spans="2:11" customFormat="1">
-      <c r="C147" s="7"/>
-      <c r="D147" s="6"/>
-      <c r="E147" s="5"/>
-      <c r="F147" s="8"/>
-      <c r="G147" s="1"/>
-      <c r="H147" s="2"/>
-      <c r="I147" s="4"/>
-      <c r="J147" s="3"/>
-      <c r="K147" s="10"/>
-    </row>
-    <row r="148" spans="2:11" customFormat="1">
-      <c r="C148" s="7"/>
-      <c r="D148" s="6"/>
-      <c r="E148" s="5"/>
-      <c r="F148" s="8"/>
-      <c r="G148" s="1"/>
-      <c r="H148" s="2"/>
-      <c r="I148" s="4"/>
-      <c r="J148" s="3"/>
-      <c r="K148" s="10"/>
-    </row>
-    <row r="149" spans="2:11" customFormat="1">
-      <c r="C149" s="7"/>
-      <c r="D149" s="6"/>
-      <c r="E149" s="5"/>
-      <c r="F149" s="8"/>
-      <c r="G149" s="1"/>
-      <c r="H149" s="2"/>
-      <c r="I149" s="4"/>
-      <c r="J149" s="3"/>
-      <c r="K149" s="10"/>
-    </row>
-    <row r="150" spans="2:11" customFormat="1">
-      <c r="C150" s="7"/>
-      <c r="D150" s="6"/>
-      <c r="E150" s="5"/>
-      <c r="F150" s="8"/>
-      <c r="G150" s="1"/>
-      <c r="H150" s="2"/>
-      <c r="I150" s="4"/>
-      <c r="J150" s="3"/>
-      <c r="K150" s="10"/>
-    </row>
-    <row r="151" spans="2:11" customFormat="1">
-      <c r="C151" s="7"/>
-      <c r="D151" s="6"/>
-      <c r="E151" s="5"/>
-      <c r="F151" s="8"/>
-      <c r="G151" s="1"/>
-      <c r="H151" s="2"/>
-      <c r="I151" s="4"/>
-      <c r="J151" s="3"/>
-      <c r="K151" s="10"/>
-    </row>
-    <row r="152" spans="2:11" customFormat="1">
-      <c r="C152" s="7"/>
-      <c r="D152" s="6"/>
-      <c r="E152" s="5"/>
-      <c r="F152" s="8"/>
-      <c r="G152" s="1"/>
-      <c r="H152" s="2"/>
-      <c r="I152" s="4"/>
-      <c r="J152" s="3"/>
-      <c r="K152" s="10"/>
-    </row>
-    <row r="153" spans="2:11" customFormat="1">
-      <c r="C153" s="7"/>
-      <c r="D153" s="6"/>
-      <c r="E153" s="5"/>
-      <c r="F153" s="8"/>
-      <c r="G153" s="1"/>
-      <c r="H153" s="2"/>
-      <c r="I153" s="4"/>
-      <c r="J153" s="3"/>
-      <c r="K153" s="10"/>
-    </row>
-    <row r="154" spans="2:11" customFormat="1">
-      <c r="C154" s="7"/>
-      <c r="D154" s="6"/>
-      <c r="E154" s="5"/>
-      <c r="F154" s="8"/>
-      <c r="G154" s="1"/>
-      <c r="H154" s="2"/>
-      <c r="I154" s="4"/>
-      <c r="J154" s="3"/>
-      <c r="K154" s="10"/>
-    </row>
-    <row r="155" spans="2:11" customFormat="1">
-      <c r="C155" s="7"/>
-      <c r="D155" s="6"/>
-      <c r="E155" s="5"/>
-      <c r="F155" s="8"/>
-      <c r="G155" s="1"/>
-      <c r="H155" s="2"/>
-      <c r="I155" s="4"/>
-      <c r="J155" s="3"/>
-      <c r="K155" s="10"/>
-    </row>
-    <row r="156" spans="2:11" customFormat="1">
-      <c r="C156" s="7"/>
-      <c r="D156" s="6"/>
-      <c r="E156" s="5"/>
-      <c r="F156" s="8"/>
-      <c r="G156" s="1"/>
-      <c r="H156" s="2"/>
-      <c r="I156" s="4"/>
-      <c r="J156" s="3"/>
-      <c r="K156" s="10"/>
-    </row>
-    <row r="157" spans="2:11" customFormat="1">
-      <c r="C157" s="7"/>
-      <c r="D157" s="6"/>
-      <c r="E157" s="5"/>
-      <c r="F157" s="8"/>
-      <c r="G157" s="1"/>
-      <c r="H157" s="2"/>
-      <c r="I157" s="4"/>
-      <c r="J157" s="3"/>
-      <c r="K157" s="10"/>
-    </row>
-    <row r="158" spans="2:11" customFormat="1">
-      <c r="C158" s="7"/>
-      <c r="D158" s="6"/>
-      <c r="E158" s="5"/>
-      <c r="F158" s="8"/>
-      <c r="G158" s="1"/>
-      <c r="H158" s="2"/>
-      <c r="I158" s="4"/>
-      <c r="J158" s="3"/>
-      <c r="K158" s="10"/>
-    </row>
-    <row r="159" spans="2:11" customFormat="1">
-      <c r="C159" s="7"/>
-      <c r="D159" s="6"/>
-      <c r="E159" s="5"/>
-      <c r="F159" s="8"/>
-      <c r="G159" s="1"/>
-      <c r="H159" s="2"/>
-      <c r="I159" s="4"/>
-      <c r="J159" s="3"/>
-      <c r="K159" s="10"/>
-    </row>
-    <row r="160" spans="2:11" customFormat="1">
-      <c r="C160" s="7"/>
-      <c r="D160" s="6"/>
-      <c r="E160" s="5"/>
-      <c r="F160" s="8"/>
-      <c r="G160" s="1"/>
-      <c r="H160" s="2"/>
-      <c r="I160" s="4"/>
-      <c r="J160" s="3"/>
-      <c r="K160" s="10"/>
-    </row>
-    <row r="161" spans="2:11" customFormat="1">
-      <c r="C161" s="7"/>
-      <c r="D161" s="6"/>
-      <c r="E161" s="5"/>
-      <c r="F161" s="8"/>
-      <c r="G161" s="1"/>
-      <c r="H161" s="2"/>
-      <c r="I161" s="4"/>
-      <c r="J161" s="3"/>
-      <c r="K161" s="10"/>
-    </row>
-    <row r="162" spans="2:11" customFormat="1">
-      <c r="C162" s="7"/>
-      <c r="D162" s="6"/>
-      <c r="E162" s="5"/>
-      <c r="F162" s="8"/>
-      <c r="G162" s="1"/>
-      <c r="H162" s="2"/>
-      <c r="I162" s="4"/>
-      <c r="J162" s="3"/>
-      <c r="K162" s="10"/>
-    </row>
-    <row r="163" spans="2:11" customFormat="1">
-      <c r="C163" s="7"/>
-      <c r="D163" s="6"/>
-      <c r="E163" s="5"/>
-      <c r="F163" s="8"/>
-      <c r="G163" s="1"/>
-      <c r="H163" s="2"/>
-      <c r="I163" s="4"/>
-      <c r="J163" s="3"/>
-      <c r="K163" s="10"/>
-    </row>
-    <row r="164" spans="2:11" customFormat="1">
-      <c r="C164" s="7"/>
-      <c r="D164" s="6"/>
-      <c r="E164" s="5"/>
-      <c r="F164" s="8"/>
-      <c r="G164" s="1"/>
-      <c r="H164" s="2"/>
-      <c r="I164" s="4"/>
-      <c r="J164" s="3"/>
-      <c r="K164" s="10"/>
-    </row>
-    <row r="165" spans="2:11" customFormat="1">
-      <c r="C165" s="7"/>
-      <c r="D165" s="6"/>
-      <c r="E165" s="5"/>
-      <c r="F165" s="8"/>
-      <c r="G165" s="1"/>
-      <c r="H165" s="2"/>
-      <c r="I165" s="4"/>
-      <c r="J165" s="3"/>
-      <c r="K165" s="10"/>
-    </row>
-    <row r="166" spans="2:11" customFormat="1">
-      <c r="C166" s="7"/>
-      <c r="D166" s="6"/>
-      <c r="E166" s="5"/>
-      <c r="F166" s="8"/>
-      <c r="G166" s="1"/>
-      <c r="H166" s="2"/>
-      <c r="I166" s="4"/>
-      <c r="J166" s="3"/>
-      <c r="K166" s="10"/>
-    </row>
-    <row r="167" spans="2:11" customFormat="1">
-      <c r="C167" s="7"/>
-      <c r="D167" s="6"/>
-      <c r="E167" s="5"/>
-      <c r="F167" s="8"/>
-      <c r="G167" s="1"/>
-      <c r="H167" s="2"/>
-      <c r="I167" s="4"/>
-      <c r="J167" s="3"/>
-      <c r="K167" s="10"/>
-    </row>
-    <row r="168" spans="2:11" customFormat="1">
-      <c r="C168" s="7"/>
-      <c r="D168" s="6"/>
-      <c r="E168" s="5"/>
-      <c r="F168" s="8"/>
-      <c r="G168" s="1"/>
-      <c r="H168" s="2"/>
-      <c r="I168" s="4"/>
-      <c r="J168" s="3"/>
-      <c r="K168" s="10"/>
-    </row>
-    <row r="170" spans="2:11" customFormat="1">
-      <c r="C170" s="7"/>
-      <c r="D170" s="6"/>
-      <c r="E170" s="5"/>
-      <c r="F170" s="8"/>
-      <c r="G170" s="1"/>
-      <c r="H170" s="2"/>
-      <c r="I170" s="4"/>
-      <c r="J170" s="3"/>
-      <c r="K170" s="10"/>
-    </row>
-    <row r="171" spans="2:11" customFormat="1">
-      <c r="C171" s="7"/>
-      <c r="D171" s="6"/>
-      <c r="E171" s="5"/>
-      <c r="F171" s="8"/>
-      <c r="G171" s="1"/>
-      <c r="H171" s="2"/>
-      <c r="I171" s="4"/>
-      <c r="J171" s="3"/>
-      <c r="K171" s="10"/>
-    </row>
-    <row r="172" spans="2:11" customFormat="1">
-      <c r="C172" s="7"/>
-      <c r="D172" s="6"/>
-      <c r="E172" s="5"/>
-      <c r="F172" s="8"/>
-      <c r="G172" s="1"/>
-      <c r="H172" s="2"/>
-      <c r="I172" s="4"/>
-      <c r="J172" s="3"/>
-      <c r="K172" s="10"/>
-    </row>
-    <row r="174" spans="2:11" customFormat="1">
-      <c r="C174" s="7"/>
-      <c r="D174" s="6"/>
-      <c r="E174" s="5"/>
-      <c r="F174" s="8"/>
-      <c r="G174" s="1"/>
-      <c r="H174" s="2"/>
-      <c r="I174" s="4"/>
-      <c r="J174" s="3"/>
-      <c r="K174" s="10"/>
-    </row>
-    <row r="175" spans="2:11" customFormat="1">
-      <c r="C175" s="7"/>
-      <c r="D175" s="6"/>
-      <c r="E175" s="5"/>
-      <c r="F175" s="8"/>
-      <c r="G175" s="1"/>
-      <c r="H175" s="2"/>
-      <c r="I175" s="4"/>
-      <c r="J175" s="3"/>
-      <c r="K175" s="10"/>
-    </row>
-    <row r="176" spans="2:11" customFormat="1">
-      <c r="C176" s="7"/>
-      <c r="D176" s="6"/>
-      <c r="E176" s="5"/>
-      <c r="F176" s="8"/>
-      <c r="G176" s="1"/>
-      <c r="H176" s="2"/>
-      <c r="I176" s="4"/>
-      <c r="J176" s="3"/>
-      <c r="K176" s="10"/>
-    </row>
-    <row r="177" spans="2:11" customFormat="1">
-      <c r="C177" s="7"/>
-      <c r="D177" s="6"/>
-      <c r="E177" s="5"/>
-      <c r="F177" s="8"/>
-      <c r="G177" s="1"/>
-      <c r="H177" s="2"/>
-      <c r="I177" s="4"/>
-      <c r="J177" s="3"/>
-      <c r="K177" s="10"/>
-    </row>
-    <row r="179" spans="2:11" customFormat="1">
-      <c r="C179" s="7"/>
-      <c r="D179" s="6"/>
-      <c r="E179" s="5"/>
-      <c r="F179" s="8"/>
-      <c r="G179" s="1"/>
-      <c r="H179" s="2"/>
-      <c r="I179" s="4"/>
-      <c r="J179" s="3"/>
-      <c r="K179" s="10"/>
-    </row>
-    <row r="180" spans="2:11" customFormat="1">
-      <c r="C180" s="7"/>
-      <c r="D180" s="6"/>
-      <c r="E180" s="5"/>
-      <c r="F180" s="8"/>
-      <c r="G180" s="1"/>
-      <c r="H180" s="2"/>
-      <c r="I180" s="4"/>
-      <c r="J180" s="3"/>
-      <c r="K180" s="10"/>
-    </row>
-    <row r="181" spans="2:11" customFormat="1">
-      <c r="C181" s="7"/>
-      <c r="D181" s="6"/>
-      <c r="E181" s="5"/>
-      <c r="F181" s="8"/>
-      <c r="G181" s="1"/>
-      <c r="H181" s="2"/>
-      <c r="I181" s="4"/>
-      <c r="J181" s="3"/>
-      <c r="K181" s="10"/>
-    </row>
-    <row r="182" spans="2:11" customFormat="1">
-      <c r="C182" s="7"/>
-      <c r="D182" s="6"/>
-      <c r="E182" s="5"/>
-      <c r="F182" s="8"/>
-      <c r="G182" s="1"/>
-      <c r="H182" s="2"/>
-      <c r="I182" s="4"/>
-      <c r="J182" s="3"/>
-      <c r="K182" s="10"/>
-    </row>
-    <row r="183" spans="2:11" customFormat="1">
-      <c r="C183" s="7"/>
-      <c r="D183" s="6"/>
-      <c r="E183" s="5"/>
-      <c r="F183" s="8"/>
-      <c r="G183" s="1"/>
-      <c r="H183" s="2"/>
-      <c r="I183" s="4"/>
-      <c r="J183" s="3"/>
-      <c r="K183" s="10"/>
-    </row>
-    <row r="184" spans="2:11" customFormat="1">
-      <c r="C184" s="7"/>
-      <c r="D184" s="6"/>
-      <c r="E184" s="5"/>
-      <c r="F184" s="8"/>
-      <c r="G184" s="1"/>
-      <c r="H184" s="2"/>
-      <c r="I184" s="4"/>
-      <c r="J184" s="3"/>
-      <c r="K184" s="10"/>
-    </row>
-    <row r="185" spans="2:11" customFormat="1">
-      <c r="C185" s="7"/>
-      <c r="D185" s="6"/>
-      <c r="E185" s="5"/>
-      <c r="F185" s="8"/>
-      <c r="G185" s="1"/>
-      <c r="H185" s="2"/>
-      <c r="I185" s="4"/>
-      <c r="J185" s="3"/>
-      <c r="K185" s="10"/>
-    </row>
-    <row r="186" spans="2:11" customFormat="1">
-      <c r="C186" s="7"/>
-      <c r="D186" s="6"/>
-      <c r="E186" s="5"/>
-      <c r="F186" s="8"/>
-      <c r="G186" s="1"/>
-      <c r="H186" s="2"/>
-      <c r="I186" s="4"/>
-      <c r="J186" s="3"/>
-      <c r="K186" s="10"/>
-    </row>
-    <row r="187" spans="2:11" customFormat="1">
-      <c r="C187" s="7"/>
-      <c r="D187" s="6"/>
-      <c r="E187" s="5"/>
-      <c r="F187" s="8"/>
-      <c r="G187" s="1"/>
-      <c r="H187" s="2"/>
-      <c r="I187" s="4"/>
-      <c r="J187" s="3"/>
-      <c r="K187" s="10"/>
-    </row>
-    <row r="188" spans="2:11" customFormat="1">
-      <c r="C188" s="7"/>
-      <c r="D188" s="6"/>
-      <c r="E188" s="5"/>
-      <c r="F188" s="8"/>
-      <c r="G188" s="1"/>
-      <c r="H188" s="2"/>
-      <c r="I188" s="4"/>
-      <c r="J188" s="3"/>
-      <c r="K188" s="10"/>
-    </row>
-    <row r="189" spans="2:11" customFormat="1">
-      <c r="C189" s="7"/>
-      <c r="D189" s="6"/>
-      <c r="E189" s="5"/>
-      <c r="F189" s="8"/>
-      <c r="G189" s="1"/>
-      <c r="H189" s="2"/>
-      <c r="I189" s="4"/>
-      <c r="J189" s="3"/>
-      <c r="K189" s="10"/>
-    </row>
-    <row r="191" spans="2:11" customFormat="1">
-      <c r="C191" s="7"/>
-      <c r="D191" s="6"/>
-      <c r="E191" s="5"/>
-      <c r="F191" s="8"/>
-      <c r="G191" s="1"/>
-      <c r="H191" s="2"/>
-      <c r="I191" s="4"/>
-      <c r="J191" s="3"/>
-      <c r="K191" s="10"/>
-    </row>
-    <row r="193" spans="2:11" customFormat="1">
-      <c r="C193" s="7"/>
-      <c r="D193" s="6"/>
-      <c r="E193" s="5"/>
-      <c r="F193" s="8"/>
-      <c r="G193" s="1"/>
-      <c r="H193" s="2"/>
-      <c r="I193" s="4"/>
-      <c r="J193" s="3"/>
-      <c r="K193" s="10"/>
-    </row>
-    <row r="195" spans="2:11" customFormat="1">
-      <c r="C195" s="7"/>
-      <c r="D195" s="6"/>
-      <c r="E195" s="5"/>
-      <c r="F195" s="8"/>
-      <c r="G195" s="1"/>
-      <c r="H195" s="2"/>
-      <c r="I195" s="4"/>
-      <c r="J195" s="3"/>
-      <c r="K195" s="10"/>
-    </row>
-    <row r="197" spans="2:11" customFormat="1">
-      <c r="C197" s="7"/>
-      <c r="D197" s="6"/>
-      <c r="E197" s="5"/>
-      <c r="F197" s="8"/>
-      <c r="G197" s="1"/>
-      <c r="H197" s="2"/>
-      <c r="I197" s="4"/>
-      <c r="J197" s="3"/>
-      <c r="K197" s="10"/>
-    </row>
-    <row r="199" spans="2:11" customFormat="1">
-      <c r="C199" s="7"/>
-      <c r="D199" s="6"/>
-      <c r="E199" s="5"/>
-      <c r="F199" s="8"/>
-      <c r="G199" s="1"/>
-      <c r="H199" s="2"/>
-      <c r="I199" s="4"/>
-      <c r="J199" s="3"/>
-      <c r="K199" s="10"/>
-    </row>
-    <row r="200" spans="2:11" customFormat="1">
-      <c r="C200" s="7"/>
-      <c r="D200" s="6"/>
-      <c r="E200" s="5"/>
-      <c r="F200" s="8"/>
-      <c r="G200" s="1"/>
-      <c r="H200" s="2"/>
-      <c r="I200" s="4"/>
-      <c r="J200" s="3"/>
-      <c r="K200" s="10"/>
-    </row>
-    <row r="201" spans="2:11" customFormat="1">
-      <c r="C201" s="7"/>
-      <c r="D201" s="6"/>
-      <c r="E201" s="5"/>
-      <c r="F201" s="8"/>
-      <c r="G201" s="1"/>
-      <c r="H201" s="2"/>
-      <c r="I201" s="4"/>
-      <c r="J201" s="3"/>
-      <c r="K201" s="10"/>
-    </row>
-    <row r="203" spans="2:11" customFormat="1">
-      <c r="C203" s="7"/>
-      <c r="D203" s="6"/>
-      <c r="E203" s="5"/>
-      <c r="F203" s="8"/>
-      <c r="G203" s="1"/>
-      <c r="H203" s="2"/>
-      <c r="I203" s="4"/>
-      <c r="J203" s="3"/>
-      <c r="K203" s="10"/>
-    </row>
-    <row r="205" spans="2:11" customFormat="1">
-      <c r="C205" s="7"/>
-      <c r="D205" s="6"/>
-      <c r="E205" s="5"/>
-      <c r="F205" s="8"/>
-      <c r="G205" s="1"/>
-      <c r="H205" s="2"/>
-      <c r="I205" s="4"/>
-      <c r="J205" s="3"/>
-      <c r="K205" s="10"/>
-    </row>
-    <row r="207" spans="2:11" customFormat="1">
-      <c r="C207" s="7"/>
-      <c r="D207" s="6"/>
-      <c r="E207" s="5"/>
-      <c r="F207" s="8"/>
-      <c r="G207" s="1"/>
-      <c r="H207" s="2"/>
-      <c r="I207" s="4"/>
-      <c r="J207" s="3"/>
-      <c r="K207" s="10"/>
-    </row>
-    <row r="209" spans="2:11" customFormat="1">
-      <c r="C209" s="7"/>
-      <c r="D209" s="6"/>
-      <c r="E209" s="5"/>
-      <c r="F209" s="8"/>
-      <c r="G209" s="1"/>
-      <c r="H209" s="2"/>
-      <c r="I209" s="4"/>
-      <c r="J209" s="3"/>
-      <c r="K209" s="10"/>
-    </row>
-    <row r="210" spans="2:11" customFormat="1">
-      <c r="C210" s="7"/>
-      <c r="D210" s="6"/>
-      <c r="E210" s="5"/>
-      <c r="F210" s="8"/>
-      <c r="G210" s="1"/>
-      <c r="H210" s="2"/>
-      <c r="I210" s="4"/>
-      <c r="J210" s="3"/>
-      <c r="K210" s="10"/>
-    </row>
-    <row r="211" spans="2:11" customFormat="1">
-      <c r="C211" s="7"/>
-      <c r="D211" s="6"/>
-      <c r="E211" s="5"/>
-      <c r="F211" s="8"/>
-      <c r="G211" s="1"/>
-      <c r="H211" s="2"/>
-      <c r="I211" s="4"/>
-      <c r="J211" s="3"/>
-      <c r="K211" s="10"/>
-    </row>
-    <row r="212" spans="2:11" customFormat="1">
-      <c r="C212" s="7"/>
-      <c r="D212" s="6"/>
-      <c r="E212" s="5"/>
-      <c r="F212" s="8"/>
-      <c r="G212" s="1"/>
-      <c r="H212" s="2"/>
-      <c r="I212" s="4"/>
-      <c r="J212" s="3"/>
-      <c r="K212" s="10"/>
-    </row>
-    <row r="213" spans="2:11" customFormat="1">
-      <c r="C213" s="7"/>
-      <c r="D213" s="6"/>
-      <c r="E213" s="5"/>
-      <c r="F213" s="8"/>
-      <c r="G213" s="1"/>
-      <c r="H213" s="2"/>
-      <c r="I213" s="4"/>
-      <c r="J213" s="3"/>
-      <c r="K213" s="10"/>
-    </row>
-    <row r="214" spans="2:11" customFormat="1">
-      <c r="C214" s="7"/>
-      <c r="D214" s="6"/>
-      <c r="E214" s="5"/>
-      <c r="F214" s="8"/>
-      <c r="G214" s="1"/>
-      <c r="H214" s="2"/>
-      <c r="I214" s="4"/>
-      <c r="J214" s="3"/>
-      <c r="K214" s="10"/>
-    </row>
-    <row r="215" spans="2:11" customFormat="1">
-      <c r="C215" s="7"/>
-      <c r="D215" s="6"/>
-      <c r="E215" s="5"/>
-      <c r="F215" s="8"/>
-      <c r="G215" s="1"/>
-      <c r="H215" s="2"/>
-      <c r="I215" s="4"/>
-      <c r="J215" s="3"/>
-      <c r="K215" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sons attaques special des persos + missions BOSS + noms des sorts des BOSS + items d'or pour chaque perso + augmentation de la vie des BOSS
</commit_message>
<xml_diff>
--- a/LeTerrain-LeJeu/src/main/resources/fichiers/personnages.xlsx
+++ b/LeTerrain-LeJeu/src/main/resources/fichiers/personnages.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19965" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="27630" windowHeight="11010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
   <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="294">
   <si>
     <t>Surnoms :</t>
   </si>
@@ -583,6 +583,324 @@
   </si>
   <si>
     <t>Ali, Alaï, l'arabe, l'arabinou de café, la pedoula, le teteur fou, Red Sugar le Diplomic</t>
+  </si>
+  <si>
+    <t>ANIMAL</t>
+  </si>
+  <si>
+    <t>FILM</t>
+  </si>
+  <si>
+    <t>SPORT</t>
+  </si>
+  <si>
+    <t>CHANTEUR</t>
+  </si>
+  <si>
+    <t>MUSIQUE</t>
+  </si>
+  <si>
+    <t>GROUPE DE MUSIQUE</t>
+  </si>
+  <si>
+    <t>JEU VIDEO</t>
+  </si>
+  <si>
+    <t>PERSONNAGE DE FILM</t>
+  </si>
+  <si>
+    <t>PERSONNAGE DE JEU VIDEO</t>
+  </si>
+  <si>
+    <t>Serpent</t>
+  </si>
+  <si>
+    <t>Freddy Mercury</t>
+  </si>
+  <si>
+    <t>Pussy Cat Dolls</t>
+  </si>
+  <si>
+    <t>FIFA/PES/GTA</t>
+  </si>
+  <si>
+    <t>Rocky Balboa</t>
+  </si>
+  <si>
+    <t>SPORTIF</t>
+  </si>
+  <si>
+    <t>Zinedine Zidane</t>
+  </si>
+  <si>
+    <t>Lady Gaga</t>
+  </si>
+  <si>
+    <t>Daft Punk</t>
+  </si>
+  <si>
+    <t>The Supermen Lovers - Starlight</t>
+  </si>
+  <si>
+    <t>Aigle</t>
+  </si>
+  <si>
+    <t>Elephant</t>
+  </si>
+  <si>
+    <t>Tortue</t>
+  </si>
+  <si>
+    <t>Eve - Ladies</t>
+  </si>
+  <si>
+    <t>De La Soul</t>
+  </si>
+  <si>
+    <t>Jennifer Lopez</t>
+  </si>
+  <si>
+    <t>Let me be a Drag Queen, Bailando</t>
+  </si>
+  <si>
+    <t>G-Squad</t>
+  </si>
+  <si>
+    <t>Snoop Dog</t>
+  </si>
+  <si>
+    <t>What's the difference between me and you - Dr Dre / Eminem</t>
+  </si>
+  <si>
+    <t>Black eyed peas</t>
+  </si>
+  <si>
+    <t>Kurt Cobain</t>
+  </si>
+  <si>
+    <t>Radiohead / Coldplay</t>
+  </si>
+  <si>
+    <t>Les Chroniques de Riddick</t>
+  </si>
+  <si>
+    <t>L'Histoire sans fin</t>
+  </si>
+  <si>
+    <t>Tigre et Dragon</t>
+  </si>
+  <si>
+    <t>Alien</t>
+  </si>
+  <si>
+    <t>Les 3 frères</t>
+  </si>
+  <si>
+    <t>Star wars</t>
+  </si>
+  <si>
+    <t>Le parrain</t>
+  </si>
+  <si>
+    <t>Indiana Jones</t>
+  </si>
+  <si>
+    <t>Lara Croft</t>
+  </si>
+  <si>
+    <t>Blood</t>
+  </si>
+  <si>
+    <t>Secret of Mana</t>
+  </si>
+  <si>
+    <t>Joe T.</t>
+  </si>
+  <si>
+    <t>Maniac Mansion</t>
+  </si>
+  <si>
+    <t>Super Mario Bros. 3</t>
+  </si>
+  <si>
+    <t>Star Wars</t>
+  </si>
+  <si>
+    <t>Dragon Ball</t>
+  </si>
+  <si>
+    <t>Princesse Aleïa</t>
+  </si>
+  <si>
+    <t>Les Guy-woks</t>
+  </si>
+  <si>
+    <t>Jobba le Hut</t>
+  </si>
+  <si>
+    <t>Cyborg C3-Pierrot</t>
+  </si>
+  <si>
+    <t>DAR2D2 / Thomanakin</t>
+  </si>
+  <si>
+    <t>Nicolhan Solo</t>
+  </si>
+  <si>
+    <t>Maitre Yoda /  Yohanakin</t>
+  </si>
+  <si>
+    <t>Obi Yan Kenobi / Yanakin / Maitre Yada</t>
+  </si>
+  <si>
+    <t>Pouvoir Dragon Ball</t>
+  </si>
+  <si>
+    <t>Kralin (Krilin)</t>
+  </si>
+  <si>
+    <t>San Guyku (San Goku)</t>
+  </si>
+  <si>
+    <t>San Johan (San Gohan)</t>
+  </si>
+  <si>
+    <t>Jojovich (Spopovich)</t>
+  </si>
+  <si>
+    <t>Nicolo (Picolo / Satan petit coeur)</t>
+  </si>
+  <si>
+    <t>Cell-main</t>
+  </si>
+  <si>
+    <t>Vegetoma / Viergeta / Tomtue Géniale</t>
+  </si>
+  <si>
+    <t>Yamcha</t>
+  </si>
+  <si>
+    <t>A des problèmes avec son nez , A un point d'indou sur le front, Finira par se marier avec une cyborg</t>
+  </si>
+  <si>
+    <t>Morsure du soleil -&gt; Bouchée du couché de soleil</t>
+  </si>
+  <si>
+    <t>La technique de l'homme bourré</t>
+  </si>
+  <si>
+    <t>Montre sa bite, Aime les serpents, Ingurgite</t>
+  </si>
+  <si>
+    <t>Points communs DB</t>
+  </si>
+  <si>
+    <t>Kamehamehaaaarg, Masenko -&gt; Malax Sen Kouille</t>
+  </si>
+  <si>
+    <t>A sauver la planete dans l'anonymat</t>
+  </si>
+  <si>
+    <t>Mon père c'est John Spopovich</t>
+  </si>
+  <si>
+    <t>Humilie une meuf en public, S'est laisser entrainer dans le coté obscur pour avoir de la masse musculaire</t>
+  </si>
+  <si>
+    <t>La technique du bras grappin extensible</t>
+  </si>
+  <si>
+    <t>Peut devenir grand mais ne le fait que rarement</t>
+  </si>
+  <si>
+    <t>Voyage dans le temps avec l'almarak</t>
+  </si>
+  <si>
+    <t>Peut manger avec sa queue des hommes et cyborgs</t>
+  </si>
+  <si>
+    <t>Solution Final Flash</t>
+  </si>
+  <si>
+    <t>La technique du Loup -&gt; La technique du Louveteau</t>
+  </si>
+  <si>
+    <t>A la même coupe de cheveux que M</t>
+  </si>
+  <si>
+    <t>Se fera transpercer le cœur et en gardera une cicatrice indelebile</t>
+  </si>
+  <si>
+    <t>Football</t>
+  </si>
+  <si>
+    <t>Escalade</t>
+  </si>
+  <si>
+    <t>Ping Pong</t>
+  </si>
+  <si>
+    <t>Natation</t>
+  </si>
+  <si>
+    <t>Cricket</t>
+  </si>
+  <si>
+    <t>Karate</t>
+  </si>
+  <si>
+    <t>Pencak-Silat</t>
+  </si>
+  <si>
+    <t>Ours</t>
+  </si>
+  <si>
+    <t>La buvette</t>
+  </si>
+  <si>
+    <t>ACTEUR</t>
+  </si>
+  <si>
+    <t>Ben Stiller</t>
+  </si>
+  <si>
+    <t>Robert De Niro</t>
+  </si>
+  <si>
+    <t>Worms Armageddon / FORZA</t>
+  </si>
+  <si>
+    <t>SERIE</t>
+  </si>
+  <si>
+    <t>Mac Gyver</t>
+  </si>
+  <si>
+    <t>Charmed</t>
+  </si>
+  <si>
+    <t>Raphael Nadal</t>
+  </si>
+  <si>
+    <t>Ian Thorpe</t>
+  </si>
+  <si>
+    <t>Kimi Räikkönen</t>
+  </si>
+  <si>
+    <t>Nickelback - How You Remind Me</t>
+  </si>
+  <si>
+    <t>Daniel Guichard - Mon Vieux</t>
+  </si>
+  <si>
+    <t>ALBUM MUSIQUE</t>
+  </si>
+  <si>
+    <t>Chroniques 2001</t>
+  </si>
+  <si>
+    <t>Dangerous</t>
   </si>
 </sst>
 </file>
@@ -807,7 +1125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -946,6 +1264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1240,17 +1559,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:K70"/>
+  <dimension ref="B1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" style="5" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" style="8" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" style="1" customWidth="1"/>
@@ -1882,7 +2201,7 @@
       <c r="J28" s="18"/>
       <c r="K28" s="36"/>
     </row>
-    <row r="29" spans="2:11" s="9" customFormat="1" ht="30">
+    <row r="29" spans="2:11" s="9" customFormat="1">
       <c r="B29" s="35" t="s">
         <v>7</v>
       </c>
@@ -2002,7 +2321,7 @@
       </c>
       <c r="K32" s="36"/>
     </row>
-    <row r="33" spans="2:11" s="9" customFormat="1" ht="30">
+    <row r="33" spans="2:11" s="9" customFormat="1">
       <c r="B33" s="35" t="s">
         <v>12</v>
       </c>
@@ -2092,7 +2411,7 @@
       </c>
       <c r="K35" s="36"/>
     </row>
-    <row r="36" spans="2:11" s="9" customFormat="1" ht="30">
+    <row r="36" spans="2:11" s="9" customFormat="1">
       <c r="B36" s="35" t="s">
         <v>13</v>
       </c>
@@ -2394,7 +2713,7 @@
       <c r="J51" s="18"/>
       <c r="K51" s="36"/>
     </row>
-    <row r="52" spans="2:11" s="9" customFormat="1" ht="45">
+    <row r="52" spans="2:11" s="9" customFormat="1" ht="45.75" thickBot="1">
       <c r="B52" s="35"/>
       <c r="C52" s="11"/>
       <c r="D52" s="12"/>
@@ -2408,175 +2727,343 @@
       <c r="J52" s="18"/>
       <c r="K52" s="36"/>
     </row>
-    <row r="53" spans="2:11" s="9" customFormat="1">
-      <c r="B53" s="35"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="16"/>
-      <c r="I53" s="17"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="36"/>
+    <row r="53" spans="2:11" s="60" customFormat="1">
+      <c r="B53" s="50"/>
+      <c r="C53" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="G53" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="H53" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="I53" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="J53" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="K53" s="59" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="54" spans="2:11" s="9" customFormat="1">
-      <c r="B54" s="35"/>
+      <c r="B54" s="35" t="s">
+        <v>188</v>
+      </c>
       <c r="C54" s="11"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="14"/>
+      <c r="D54" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>277</v>
+      </c>
       <c r="G54" s="15"/>
-      <c r="H54" s="16"/>
-      <c r="I54" s="17"/>
+      <c r="H54" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="I54" s="17" t="s">
+        <v>209</v>
+      </c>
       <c r="J54" s="18"/>
       <c r="K54" s="36"/>
     </row>
     <row r="55" spans="2:11" s="9" customFormat="1">
-      <c r="B55" s="35"/>
+      <c r="B55" s="35" t="s">
+        <v>279</v>
+      </c>
       <c r="C55" s="11"/>
-      <c r="D55" s="12"/>
+      <c r="D55" s="19" t="s">
+        <v>281</v>
+      </c>
       <c r="E55" s="13"/>
       <c r="F55" s="14"/>
       <c r="G55" s="15"/>
       <c r="H55" s="16"/>
-      <c r="I55" s="17"/>
+      <c r="I55" s="17" t="s">
+        <v>280</v>
+      </c>
       <c r="J55" s="18"/>
       <c r="K55" s="36"/>
     </row>
     <row r="56" spans="2:11" s="9" customFormat="1">
-      <c r="B56" s="35"/>
+      <c r="B56" s="35" t="s">
+        <v>189</v>
+      </c>
       <c r="C56" s="11"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="15"/>
-      <c r="H56" s="16"/>
-      <c r="I56" s="17"/>
-      <c r="J56" s="18"/>
+      <c r="D56" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="G56" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="H56" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="I56" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="J56" s="18" t="s">
+        <v>225</v>
+      </c>
       <c r="K56" s="36"/>
     </row>
-    <row r="57" spans="2:11" s="9" customFormat="1">
-      <c r="B57" s="35"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="15"/>
-      <c r="H57" s="16"/>
-      <c r="I57" s="17"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="36"/>
+    <row r="57" spans="2:11" customFormat="1">
+      <c r="B57" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="C57" s="27"/>
+      <c r="D57" s="66" t="s">
+        <v>227</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F57" s="30"/>
+      <c r="G57" s="31"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="34"/>
+      <c r="K57" s="39"/>
     </row>
     <row r="58" spans="2:11" s="9" customFormat="1">
-      <c r="B58" s="35"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="15"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="17"/>
-      <c r="J58" s="18"/>
+      <c r="B58" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="G58" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="H58" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="I58" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="J58" s="18" t="s">
+        <v>271</v>
+      </c>
       <c r="K58" s="36"/>
     </row>
     <row r="59" spans="2:11" s="9" customFormat="1">
-      <c r="B59" s="35"/>
+      <c r="B59" s="35" t="s">
+        <v>202</v>
+      </c>
       <c r="C59" s="11"/>
       <c r="D59" s="12"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="15"/>
+      <c r="E59" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="G59" s="15" t="s">
+        <v>286</v>
+      </c>
       <c r="H59" s="16"/>
       <c r="I59" s="17"/>
-      <c r="J59" s="18"/>
+      <c r="J59" s="18" t="s">
+        <v>288</v>
+      </c>
       <c r="K59" s="36"/>
     </row>
     <row r="60" spans="2:11" s="9" customFormat="1">
-      <c r="B60" s="35"/>
+      <c r="B60" s="35" t="s">
+        <v>283</v>
+      </c>
       <c r="C60" s="11"/>
       <c r="D60" s="12"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="14"/>
+      <c r="E60" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="F60" s="14" t="s">
+        <v>285</v>
+      </c>
       <c r="G60" s="15"/>
       <c r="H60" s="16"/>
-      <c r="I60" s="17"/>
-      <c r="J60" s="18"/>
+      <c r="I60" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="J60" s="18" t="s">
+        <v>46</v>
+      </c>
       <c r="K60" s="36"/>
     </row>
-    <row r="61" spans="2:11">
-      <c r="B61" s="38"/>
-      <c r="C61" s="27"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="29"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="31"/>
-      <c r="H61" s="32"/>
-      <c r="I61" s="33"/>
-      <c r="J61" s="34"/>
-      <c r="K61" s="39"/>
-    </row>
-    <row r="62" spans="2:11">
-      <c r="B62" s="38"/>
-      <c r="C62" s="27"/>
-      <c r="D62" s="28"/>
-      <c r="E62" s="29"/>
-      <c r="F62" s="30"/>
-      <c r="G62" s="31"/>
-      <c r="H62" s="32"/>
-      <c r="I62" s="33"/>
-      <c r="J62" s="34"/>
-      <c r="K62" s="39"/>
-    </row>
-    <row r="63" spans="2:11">
-      <c r="B63" s="38"/>
-      <c r="C63" s="27"/>
-      <c r="D63" s="28"/>
-      <c r="E63" s="29"/>
-      <c r="F63" s="30"/>
-      <c r="G63" s="31"/>
-      <c r="H63" s="32"/>
-      <c r="I63" s="33"/>
-      <c r="J63" s="34"/>
-      <c r="K63" s="39"/>
-    </row>
-    <row r="64" spans="2:11">
-      <c r="B64" s="38"/>
-      <c r="C64" s="27"/>
-      <c r="D64" s="28"/>
-      <c r="E64" s="29"/>
-      <c r="F64" s="30"/>
-      <c r="G64" s="31"/>
-      <c r="H64" s="32"/>
-      <c r="I64" s="33"/>
-      <c r="J64" s="34"/>
-      <c r="K64" s="39"/>
-    </row>
-    <row r="65" spans="2:11">
-      <c r="B65" s="38"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="28"/>
-      <c r="E65" s="29"/>
-      <c r="F65" s="30"/>
-      <c r="G65" s="31"/>
-      <c r="H65" s="32"/>
-      <c r="I65" s="33"/>
-      <c r="J65" s="34"/>
-      <c r="K65" s="39"/>
-    </row>
-    <row r="66" spans="2:11">
-      <c r="B66" s="38"/>
+    <row r="61" spans="2:11" s="9" customFormat="1">
+      <c r="B61" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="F61" s="14"/>
+      <c r="G61" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="H61" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="I61" s="17"/>
+      <c r="J61" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="K61" s="36"/>
+    </row>
+    <row r="62" spans="2:11" s="9" customFormat="1" ht="45">
+      <c r="B62" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="G62" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="H62" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="I62" s="17"/>
+      <c r="J62" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="K62" s="36"/>
+    </row>
+    <row r="63" spans="2:11" s="9" customFormat="1">
+      <c r="B63" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="C63" s="11"/>
+      <c r="D63" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="E63" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="G63" s="15"/>
+      <c r="H63" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="I63" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="J63" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="K63" s="36"/>
+    </row>
+    <row r="64" spans="2:11" s="9" customFormat="1">
+      <c r="B64" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="C64" s="11"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="H64" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="I64" s="17"/>
+      <c r="J64" s="18"/>
+      <c r="K64" s="36"/>
+    </row>
+    <row r="65" spans="2:11" s="9" customFormat="1" ht="30">
+      <c r="B65" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="C65" s="11"/>
+      <c r="D65" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G65" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="H65" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="I65" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="J65" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="K65" s="36"/>
+    </row>
+    <row r="66" spans="2:11" customFormat="1">
+      <c r="B66" s="38" t="s">
+        <v>196</v>
+      </c>
       <c r="C66" s="27"/>
       <c r="D66" s="28"/>
       <c r="E66" s="29"/>
-      <c r="F66" s="30"/>
-      <c r="G66" s="31"/>
+      <c r="F66" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="G66" s="31" t="s">
+        <v>228</v>
+      </c>
       <c r="H66" s="32"/>
       <c r="I66" s="33"/>
       <c r="J66" s="34"/>
       <c r="K66" s="39"/>
     </row>
-    <row r="67" spans="2:11">
+    <row r="67" spans="2:11" customFormat="1">
       <c r="B67" s="38"/>
       <c r="C67" s="27"/>
       <c r="D67" s="28"/>
@@ -2588,41 +3075,184 @@
       <c r="J67" s="34"/>
       <c r="K67" s="39"/>
     </row>
-    <row r="68" spans="2:11">
-      <c r="B68" s="38"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="28"/>
-      <c r="E68" s="29"/>
-      <c r="F68" s="30"/>
-      <c r="G68" s="31"/>
-      <c r="H68" s="32"/>
-      <c r="I68" s="33"/>
-      <c r="J68" s="34"/>
+    <row r="68" spans="2:11" customFormat="1">
+      <c r="B68" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="C68" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="D68" s="66" t="s">
+        <v>237</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="F68" s="30" t="s">
+        <v>238</v>
+      </c>
+      <c r="G68" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="H68" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="I68" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="J68" s="34" t="s">
+        <v>243</v>
+      </c>
       <c r="K68" s="39"/>
     </row>
-    <row r="69" spans="2:11">
-      <c r="B69" s="38"/>
-      <c r="C69" s="27"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="29"/>
-      <c r="F69" s="30"/>
-      <c r="G69" s="31"/>
-      <c r="H69" s="32"/>
-      <c r="I69" s="33"/>
-      <c r="J69" s="34"/>
+    <row r="69" spans="2:11" customFormat="1">
+      <c r="B69" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="C69" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="D69" s="66" t="s">
+        <v>246</v>
+      </c>
+      <c r="E69" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="F69" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="G69" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="H69" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="I69" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="J69" s="34" t="s">
+        <v>252</v>
+      </c>
       <c r="K69" s="39"/>
     </row>
-    <row r="70" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B70" s="40"/>
-      <c r="C70" s="41"/>
-      <c r="D70" s="42"/>
-      <c r="E70" s="43"/>
-      <c r="F70" s="44"/>
-      <c r="G70" s="45"/>
-      <c r="H70" s="46"/>
-      <c r="I70" s="47"/>
-      <c r="J70" s="48"/>
-      <c r="K70" s="49"/>
+    <row r="70" spans="2:11" customFormat="1">
+      <c r="B70" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="C70" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="D70" s="66" t="s">
+        <v>255</v>
+      </c>
+      <c r="E70" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="F70" s="30" t="s">
+        <v>260</v>
+      </c>
+      <c r="G70" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="H70" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="I70" s="33" t="s">
+        <v>266</v>
+      </c>
+      <c r="J70" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="K70" s="39"/>
+    </row>
+    <row r="71" spans="2:11" customFormat="1">
+      <c r="B71" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="C71" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="D71" s="66" t="s">
+        <v>256</v>
+      </c>
+      <c r="E71" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="F71" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="G71" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="H71" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="I71" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="J71" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="K71" s="39"/>
+    </row>
+    <row r="72" spans="2:11" customFormat="1">
+      <c r="B72" s="38"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="30"/>
+      <c r="G72" s="31"/>
+      <c r="H72" s="32"/>
+      <c r="I72" s="33"/>
+      <c r="J72" s="34"/>
+      <c r="K72" s="39"/>
+    </row>
+    <row r="73" spans="2:11" customFormat="1">
+      <c r="B73" s="38"/>
+      <c r="C73" s="27"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="29"/>
+      <c r="F73" s="30"/>
+      <c r="G73" s="31"/>
+      <c r="H73" s="32"/>
+      <c r="I73" s="33"/>
+      <c r="J73" s="34"/>
+      <c r="K73" s="39"/>
+    </row>
+    <row r="74" spans="2:11" customFormat="1">
+      <c r="B74" s="38"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="30"/>
+      <c r="G74" s="31"/>
+      <c r="H74" s="32"/>
+      <c r="I74" s="33"/>
+      <c r="J74" s="34"/>
+      <c r="K74" s="39"/>
+    </row>
+    <row r="75" spans="2:11" customFormat="1" ht="15.75" thickBot="1">
+      <c r="B75" s="40"/>
+      <c r="C75" s="41"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="43"/>
+      <c r="F75" s="44"/>
+      <c r="G75" s="45"/>
+      <c r="H75" s="46"/>
+      <c r="I75" s="47"/>
+      <c r="J75" s="48"/>
+      <c r="K75" s="49"/>
+    </row>
+    <row r="76" spans="2:11" customFormat="1">
+      <c r="C76" s="7"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="8"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Externalisation des variables de configuration dans "leTerrain.properties" + Ajout des Mini BOSS Prof + gestion des items en combat et hors combat + nom et image des ennemis aleatoire + ajout d'un sac groupe + messages Dieu au debut + musiques d'ambiances par perso + correction de bugs
</commit_message>
<xml_diff>
--- a/LeTerrain-LeJeu/src/main/resources/fichiers/personnages.xlsx
+++ b/LeTerrain-LeJeu/src/main/resources/fichiers/personnages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="27630" windowHeight="11010"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="18030" windowHeight="8625"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="295">
   <si>
     <t>Surnoms :</t>
   </si>
@@ -552,12 +552,6 @@
     <t>qu'on lui dise qu'il a des seins, qu'on chante get around des beachboys, les gens qui profite du système et des tickets restos</t>
   </si>
   <si>
-    <t>Conduit uniquement des Fiat Punto, fait encore des etudes, fait des coups de putes,  vit dans une ferme, connait Gino et ses pizzas, ne s'est jamais battu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fume sans acheter de paquet, sait faire le gitan, s'allonge sur un canape quand foncde, </t>
-  </si>
-  <si>
     <t xml:space="preserve">est nerveux parce qu'il a un corps de lache et une narine qui part en couille, porte des lunettes de bigleux, fume comme un pd la main a plat, </t>
   </si>
   <si>
@@ -750,9 +744,6 @@
     <t>Maitre Yoda /  Yohanakin</t>
   </si>
   <si>
-    <t>Obi Yan Kenobi / Yanakin / Maitre Yada</t>
-  </si>
-  <si>
     <t>Pouvoir Dragon Ball</t>
   </si>
   <si>
@@ -901,6 +892,18 @@
   </si>
   <si>
     <t>Dangerous</t>
+  </si>
+  <si>
+    <t>Obi Yan Kenobi / Yanakin / Maitre Yada / Yan solo</t>
+  </si>
+  <si>
+    <t>Mickael Jordan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fume sans acheter de paquet, sait faire l'accent gitan,sait faire l'accent quebecois, s'allonge sur un canape quand foncde, </t>
+  </si>
+  <si>
+    <t>Conduit uniquement des Fiat Punto, fait encore des etudes, fait des coups de putes,  vit dans une ferme, connait Gino et ses pizzas, ne s'est jamais battu, sait faire l'accent belge de Bruges</t>
   </si>
 </sst>
 </file>
@@ -1561,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="J64" sqref="J64"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1680,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>126</v>
@@ -1692,10 +1695,10 @@
         <v>53</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>52</v>
@@ -1766,7 +1769,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>178</v>
+        <v>293</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>116</v>
@@ -1775,7 +1778,7 @@
         <v>145</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>177</v>
+        <v>294</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>110</v>
@@ -1796,7 +1799,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>114</v>
@@ -1832,13 +1835,13 @@
         <v>115</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>173</v>
@@ -2572,7 +2575,7 @@
         <v>149</v>
       </c>
       <c r="I43" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J43" s="18" t="s">
         <v>103</v>
@@ -2659,7 +2662,7 @@
       <c r="H48" s="16"/>
       <c r="I48" s="17"/>
       <c r="J48" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K48" s="36"/>
     </row>
@@ -2759,84 +2762,84 @@
     </row>
     <row r="54" spans="2:11" s="9" customFormat="1">
       <c r="B54" s="35" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C54" s="11"/>
       <c r="D54" s="19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="16" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I54" s="17" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J54" s="18"/>
       <c r="K54" s="36"/>
     </row>
     <row r="55" spans="2:11" s="9" customFormat="1">
       <c r="B55" s="35" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C55" s="11"/>
       <c r="D55" s="19" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E55" s="13"/>
       <c r="F55" s="14"/>
       <c r="G55" s="15"/>
       <c r="H55" s="16"/>
       <c r="I55" s="17" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="J55" s="18"/>
       <c r="K55" s="36"/>
     </row>
     <row r="56" spans="2:11" s="9" customFormat="1">
       <c r="B56" s="35" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E56" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="G56" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="H56" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="F56" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="G56" s="15" t="s">
+      <c r="I56" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="H56" s="16" t="s">
+      <c r="J56" s="18" t="s">
         <v>223</v>
-      </c>
-      <c r="I56" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="J56" s="18" t="s">
-        <v>225</v>
       </c>
       <c r="K56" s="36"/>
     </row>
     <row r="57" spans="2:11" customFormat="1">
       <c r="B57" s="38" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C57" s="27"/>
       <c r="D57" s="66" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E57" s="29" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F57" s="30"/>
       <c r="G57" s="31"/>
@@ -2847,67 +2850,69 @@
     </row>
     <row r="58" spans="2:11" s="9" customFormat="1">
       <c r="B58" s="35" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D58" s="19" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E58" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="F58" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F58" s="14" t="s">
+      <c r="G58" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="G58" s="15" t="s">
-        <v>276</v>
-      </c>
       <c r="H58" s="16" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="I58" s="17" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="J58" s="18" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="K58" s="36"/>
     </row>
     <row r="59" spans="2:11" s="9" customFormat="1">
       <c r="B59" s="35" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C59" s="11"/>
       <c r="D59" s="12"/>
       <c r="E59" s="13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H59" s="16"/>
-      <c r="I59" s="17"/>
+      <c r="I59" s="17" t="s">
+        <v>292</v>
+      </c>
       <c r="J59" s="18" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="K59" s="36"/>
     </row>
     <row r="60" spans="2:11" s="9" customFormat="1">
       <c r="B60" s="35" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C60" s="11"/>
       <c r="D60" s="12"/>
       <c r="E60" s="13" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F60" s="14" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G60" s="15"/>
       <c r="H60" s="16"/>
@@ -2921,97 +2926,97 @@
     </row>
     <row r="61" spans="2:11" s="9" customFormat="1">
       <c r="B61" s="35" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>88</v>
       </c>
       <c r="D61" s="19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F61" s="14"/>
       <c r="G61" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H61" s="16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I61" s="17"/>
       <c r="J61" s="18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K61" s="36"/>
     </row>
     <row r="62" spans="2:11" s="9" customFormat="1" ht="45">
       <c r="B62" s="35" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D62" s="19" t="s">
         <v>105</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H62" s="16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I62" s="17"/>
       <c r="J62" s="18" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="K62" s="36"/>
     </row>
     <row r="63" spans="2:11" s="9" customFormat="1">
       <c r="B63" s="35" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C63" s="11"/>
       <c r="D63" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G63" s="15"/>
       <c r="H63" s="16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I63" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="J63" s="18" t="s">
         <v>217</v>
-      </c>
-      <c r="J63" s="18" t="s">
-        <v>219</v>
       </c>
       <c r="K63" s="36"/>
     </row>
     <row r="64" spans="2:11" s="9" customFormat="1">
       <c r="B64" s="35" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C64" s="11"/>
       <c r="D64" s="19"/>
       <c r="E64" s="13"/>
       <c r="F64" s="14"/>
       <c r="G64" s="15" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I64" s="17"/>
       <c r="J64" s="18"/>
@@ -3019,44 +3024,44 @@
     </row>
     <row r="65" spans="2:11" s="9" customFormat="1" ht="30">
       <c r="B65" s="35" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C65" s="11"/>
       <c r="D65" s="19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E65" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G65" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="H65" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="F65" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="G65" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="H65" s="16" t="s">
-        <v>232</v>
-      </c>
       <c r="I65" s="17" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J65" s="18" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K65" s="36"/>
     </row>
     <row r="66" spans="2:11" customFormat="1">
       <c r="B66" s="38" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C66" s="27"/>
       <c r="D66" s="28"/>
       <c r="E66" s="29"/>
       <c r="F66" s="30" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G66" s="31" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H66" s="32"/>
       <c r="I66" s="33"/>
@@ -3077,121 +3082,121 @@
     </row>
     <row r="68" spans="2:11" customFormat="1">
       <c r="B68" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="C68" s="27" t="s">
         <v>234</v>
       </c>
-      <c r="C68" s="27" t="s">
+      <c r="D68" s="66" t="s">
+        <v>235</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="F68" s="30" t="s">
         <v>236</v>
       </c>
-      <c r="D68" s="66" t="s">
+      <c r="G68" s="31" t="s">
+        <v>239</v>
+      </c>
+      <c r="H68" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="E68" s="29" t="s">
-        <v>242</v>
-      </c>
-      <c r="F68" s="30" t="s">
+      <c r="I68" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="G68" s="31" t="s">
-        <v>241</v>
-      </c>
-      <c r="H68" s="32" t="s">
-        <v>239</v>
-      </c>
-      <c r="I68" s="33" t="s">
-        <v>240</v>
-      </c>
       <c r="J68" s="34" t="s">
-        <v>243</v>
+        <v>291</v>
       </c>
       <c r="K68" s="39"/>
     </row>
     <row r="69" spans="2:11" customFormat="1">
       <c r="B69" s="38" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C69" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="D69" s="66" t="s">
+        <v>243</v>
+      </c>
+      <c r="E69" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="F69" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="D69" s="66" t="s">
+      <c r="G69" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="E69" s="29" t="s">
+      <c r="H69" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="F69" s="30" t="s">
+      <c r="I69" s="33" t="s">
         <v>248</v>
       </c>
-      <c r="G69" s="31" t="s">
+      <c r="J69" s="34" t="s">
         <v>249</v>
-      </c>
-      <c r="H69" s="32" t="s">
-        <v>250</v>
-      </c>
-      <c r="I69" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="J69" s="34" t="s">
-        <v>252</v>
       </c>
       <c r="K69" s="39"/>
     </row>
     <row r="70" spans="2:11" customFormat="1">
       <c r="B70" s="38" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C70" s="27" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D70" s="66" t="s">
+        <v>252</v>
+      </c>
+      <c r="E70" s="29" t="s">
         <v>255</v>
       </c>
-      <c r="E70" s="29" t="s">
-        <v>258</v>
-      </c>
       <c r="F70" s="30" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G70" s="31" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H70" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="I70" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="J70" s="34" t="s">
         <v>264</v>
-      </c>
-      <c r="I70" s="33" t="s">
-        <v>266</v>
-      </c>
-      <c r="J70" s="34" t="s">
-        <v>267</v>
       </c>
       <c r="K70" s="39"/>
     </row>
     <row r="71" spans="2:11" customFormat="1">
       <c r="B71" s="38" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C71" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="D71" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="D71" s="66" t="s">
+      <c r="E71" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="E71" s="29" t="s">
-        <v>259</v>
-      </c>
       <c r="F71" s="30" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G71" s="31" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="H71" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="I71" s="33" t="s">
         <v>265</v>
       </c>
-      <c r="I71" s="33" t="s">
-        <v>268</v>
-      </c>
       <c r="J71" s="34" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="K71" s="39"/>
     </row>

</xml_diff>